<commit_message>
predicting ashenfelter with predicted precip and temp
</commit_message>
<xml_diff>
--- a/data/bordeauxWeather.xlsx
+++ b/data/bordeauxWeather.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polin\Dropbox\EE 608 spring 2023\project\Wine-Quality-Modeling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A978E2B9-26E9-46D5-9EEF-187426C245CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA673005-1110-44C0-9092-1F78BA91C66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{D0F1188E-B2DB-4E86-B194-F78466D191BE}"/>
+    <workbookView xWindow="12660" yWindow="0" windowWidth="18048" windowHeight="16680" activeTab="1" xr2:uid="{D0F1188E-B2DB-4E86-B194-F78466D191BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>year</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>jun</t>
-  </si>
-  <si>
-    <t>jul</t>
-  </si>
-  <si>
-    <t>aug</t>
   </si>
   <si>
     <t>avgTempAprilSeptember</t>
@@ -69,9 +63,6 @@
     <t>mar</t>
   </si>
   <si>
-    <t>oct</t>
-  </si>
-  <si>
     <t>nov</t>
   </si>
   <si>
@@ -79,9 +70,6 @@
   </si>
   <si>
     <t>sepT</t>
-  </si>
-  <si>
-    <t>sep</t>
   </si>
   <si>
     <t>totalPSeptAug</t>
@@ -107,12 +95,39 @@
   <si>
     <t>julT</t>
   </si>
+  <si>
+    <t>augP</t>
+  </si>
+  <si>
+    <t>sepP</t>
+  </si>
+  <si>
+    <t>julP</t>
+  </si>
+  <si>
+    <t>octP</t>
+  </si>
+  <si>
+    <t>janP</t>
+  </si>
+  <si>
+    <t>febP</t>
+  </si>
+  <si>
+    <t>marP</t>
+  </si>
+  <si>
+    <t>novP</t>
+  </si>
+  <si>
+    <t>decP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +153,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,6 +361,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -377,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -487,10 +522,16 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -499,6 +540,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -809,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B54E63-F438-48F7-83CF-1118160EA2FA}">
   <dimension ref="A1:Y102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A18" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -826,37 +872,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="38" t="s">
-        <v>17</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="M1" s="35" t="s">
         <v>7</v>
-      </c>
-      <c r="L1" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="35" t="s">
-        <v>9</v>
       </c>
       <c r="N1" s="35" t="s">
         <v>1</v>
@@ -868,31 +914,31 @@
         <v>3</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="V1" s="35" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="W1" s="35" t="s">
         <v>0</v>
       </c>
       <c r="X1" s="36" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="Y1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="15" thickBot="1">
@@ -8680,525 +8726,2773 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EC36CD-A611-4488-BA35-43D34F546F10}">
-  <dimension ref="A1:A102"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="8" max="8" width="20.77734375" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" thickBot="1">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:8" ht="15" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1">
+      <c r="A2">
+        <v>1921</v>
+      </c>
+      <c r="B2" s="10">
+        <v>65</v>
+      </c>
+      <c r="C2" s="11">
+        <v>33</v>
+      </c>
+      <c r="D2" s="11">
+        <v>27</v>
+      </c>
+      <c r="E2" s="12">
+        <v>41</v>
+      </c>
+      <c r="F2" s="13">
+        <v>64</v>
+      </c>
+      <c r="G2" s="11">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <f>SUM(B2:D2)+SUM(E2:G2)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1">
+      <c r="A3">
+        <v>1922</v>
+      </c>
+      <c r="B3" s="19">
+        <v>91</v>
+      </c>
+      <c r="C3" s="11">
+        <v>29</v>
+      </c>
+      <c r="D3" s="19">
+        <v>92</v>
+      </c>
+      <c r="E3" s="17">
+        <v>8</v>
+      </c>
+      <c r="F3" s="16">
+        <v>21</v>
+      </c>
+      <c r="G3" s="18">
+        <v>48</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H66" si="0">SUM(B3:D3)+SUM(E3:G3)</f>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1">
+      <c r="A4">
+        <v>1923</v>
+      </c>
+      <c r="B4" s="10">
+        <v>65</v>
+      </c>
+      <c r="C4" s="23">
+        <v>116</v>
+      </c>
+      <c r="D4" s="24">
+        <v>82</v>
+      </c>
+      <c r="E4" s="10">
+        <v>69</v>
+      </c>
+      <c r="F4" s="18">
+        <v>48</v>
+      </c>
+      <c r="G4" s="21">
+        <v>109</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1">
+      <c r="A5">
+        <v>1924</v>
+      </c>
+      <c r="B5" s="19">
+        <v>88</v>
+      </c>
+      <c r="C5" s="12">
+        <v>42</v>
+      </c>
+      <c r="D5" s="24">
+        <v>82</v>
+      </c>
+      <c r="E5" s="13">
+        <v>58</v>
+      </c>
+      <c r="F5" s="26">
+        <v>151</v>
+      </c>
+      <c r="G5" s="27">
+        <v>169</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1">
+      <c r="A6">
+        <v>1925</v>
+      </c>
+      <c r="B6" s="12">
+        <v>36</v>
+      </c>
+      <c r="C6" s="29">
+        <v>182</v>
+      </c>
+      <c r="D6" s="11">
+        <v>32</v>
+      </c>
+      <c r="E6" s="24">
+        <v>78</v>
+      </c>
+      <c r="F6" s="19">
+        <v>92</v>
+      </c>
+      <c r="G6" s="24">
+        <v>84</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1">
+      <c r="A7">
+        <v>1926</v>
+      </c>
+      <c r="B7" s="23">
+        <v>124</v>
+      </c>
+      <c r="C7" s="19">
+        <v>87</v>
+      </c>
+      <c r="D7" s="12">
+        <v>45</v>
+      </c>
+      <c r="E7" s="24">
+        <v>80</v>
+      </c>
+      <c r="F7" s="23">
+        <v>117</v>
+      </c>
+      <c r="G7" s="18">
+        <v>49</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1">
+      <c r="A8">
+        <v>1927</v>
+      </c>
+      <c r="B8" s="15">
+        <v>100</v>
+      </c>
+      <c r="C8" s="19">
+        <v>95</v>
+      </c>
+      <c r="D8" s="31">
+        <v>206</v>
+      </c>
+      <c r="E8" s="10">
+        <v>71</v>
+      </c>
+      <c r="F8" s="22">
+        <v>158</v>
+      </c>
+      <c r="G8" s="11">
+        <v>26</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>656</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1">
+      <c r="A9">
+        <v>1928</v>
+      </c>
+      <c r="B9" s="24">
+        <v>84</v>
+      </c>
+      <c r="C9" s="19">
+        <v>92</v>
+      </c>
+      <c r="D9" s="25">
+        <v>136</v>
+      </c>
+      <c r="E9" s="16">
+        <v>19</v>
+      </c>
+      <c r="F9" s="19">
+        <v>89</v>
+      </c>
+      <c r="G9" s="10">
+        <v>72</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1">
+      <c r="A10">
+        <v>1929</v>
+      </c>
+      <c r="B10" s="17">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10">
+        <v>67</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="E10" s="23">
+        <v>120</v>
+      </c>
+      <c r="F10" s="22">
+        <v>161</v>
+      </c>
+      <c r="G10" s="15">
+        <v>99</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>460.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1">
+      <c r="A11">
+        <v>1930</v>
+      </c>
+      <c r="B11" s="15">
+        <v>101</v>
+      </c>
+      <c r="C11" s="15">
+        <v>96</v>
+      </c>
+      <c r="D11" s="25">
+        <v>137</v>
+      </c>
+      <c r="E11" s="21">
+        <v>111</v>
+      </c>
+      <c r="F11" s="21">
+        <v>109</v>
+      </c>
+      <c r="G11" s="26">
+        <v>152</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>706</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1">
+      <c r="A12">
+        <v>1931</v>
+      </c>
+      <c r="B12" s="21">
+        <v>111</v>
+      </c>
+      <c r="C12" s="23">
+        <v>117</v>
+      </c>
+      <c r="D12" s="21">
+        <v>108</v>
+      </c>
+      <c r="E12" s="29">
+        <v>178</v>
+      </c>
+      <c r="F12" s="28">
+        <v>197</v>
+      </c>
+      <c r="G12" s="22">
+        <v>156</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>867</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1">
+      <c r="A13">
+        <v>1932</v>
+      </c>
+      <c r="B13" s="18">
+        <v>51</v>
+      </c>
+      <c r="C13" s="14">
+        <v>3</v>
+      </c>
+      <c r="D13" s="24">
+        <v>78</v>
+      </c>
+      <c r="E13" s="11">
+        <v>25</v>
+      </c>
+      <c r="F13" s="26">
+        <v>154</v>
+      </c>
+      <c r="G13" s="12">
+        <v>35</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1">
+      <c r="A14">
+        <v>1933</v>
+      </c>
+      <c r="B14" s="18">
+        <v>45</v>
+      </c>
+      <c r="C14" s="19">
+        <v>88</v>
+      </c>
+      <c r="D14" s="12">
+        <v>41</v>
+      </c>
+      <c r="E14" s="29">
+        <v>178</v>
+      </c>
+      <c r="F14" s="13">
+        <v>62</v>
+      </c>
+      <c r="G14" s="11">
+        <v>31</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1">
+      <c r="A15">
+        <v>1934</v>
+      </c>
+      <c r="B15" s="13">
+        <v>63</v>
+      </c>
+      <c r="C15" s="17">
+        <v>13</v>
+      </c>
+      <c r="D15" s="29">
+        <v>182</v>
+      </c>
+      <c r="E15" s="26">
+        <v>152</v>
+      </c>
+      <c r="F15" s="13">
+        <v>64</v>
+      </c>
+      <c r="G15" s="13">
+        <v>65</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>539</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1">
+      <c r="A16">
+        <v>1935</v>
+      </c>
+      <c r="B16" s="12">
+        <v>39</v>
+      </c>
+      <c r="C16" s="25">
+        <v>142</v>
+      </c>
+      <c r="D16" s="12">
+        <v>39</v>
+      </c>
+      <c r="E16" s="18">
+        <v>55</v>
+      </c>
+      <c r="F16" s="25">
+        <v>136</v>
+      </c>
+      <c r="G16" s="22">
+        <v>165</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1">
+      <c r="A17">
+        <v>1936</v>
+      </c>
+      <c r="B17" s="25">
+        <v>144</v>
+      </c>
+      <c r="C17" s="20">
+        <v>133</v>
+      </c>
+      <c r="D17" s="12">
+        <v>44</v>
+      </c>
+      <c r="E17" s="15">
+        <v>97</v>
+      </c>
+      <c r="F17" s="26">
+        <v>150</v>
+      </c>
+      <c r="G17" s="31">
+        <v>212</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>780</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1">
+      <c r="A18">
+        <v>1937</v>
+      </c>
+      <c r="B18" s="24">
+        <v>81</v>
+      </c>
+      <c r="C18" s="23">
+        <v>117</v>
+      </c>
+      <c r="D18" s="23">
+        <v>123</v>
+      </c>
+      <c r="E18" s="16">
+        <v>20</v>
+      </c>
+      <c r="F18" s="19">
+        <v>93</v>
+      </c>
+      <c r="G18" s="11">
+        <v>25</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1">
+      <c r="A19">
+        <v>1938</v>
+      </c>
+      <c r="B19" s="21">
+        <v>113</v>
+      </c>
+      <c r="C19" s="16">
+        <v>17</v>
+      </c>
+      <c r="D19" s="17">
+        <v>11</v>
+      </c>
+      <c r="E19" s="15">
+        <v>101</v>
+      </c>
+      <c r="F19" s="19">
+        <v>91</v>
+      </c>
+      <c r="G19" s="33">
+        <v>215</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>548</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1">
+      <c r="A20">
+        <v>1939</v>
+      </c>
+      <c r="B20" s="27">
+        <v>168</v>
+      </c>
+      <c r="C20" s="11">
+        <v>31</v>
+      </c>
+      <c r="D20" s="10">
+        <v>73</v>
+      </c>
+      <c r="E20" s="13">
+        <v>60</v>
+      </c>
+      <c r="F20" s="21">
+        <v>112</v>
+      </c>
+      <c r="G20" s="19">
+        <v>93</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>537</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1">
+      <c r="A21">
+        <v>1940</v>
+      </c>
+      <c r="B21" s="12">
+        <v>42</v>
+      </c>
+      <c r="C21" s="24">
+        <v>80</v>
+      </c>
+      <c r="D21" s="18">
+        <v>53</v>
+      </c>
+      <c r="E21" s="25">
+        <v>137</v>
+      </c>
+      <c r="F21" s="19">
+        <v>86</v>
+      </c>
+      <c r="G21" s="19">
+        <v>91</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>489</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" thickBot="1">
+      <c r="A22">
+        <v>1941</v>
+      </c>
+      <c r="B22" s="19">
+        <v>92</v>
+      </c>
+      <c r="C22" s="20">
+        <v>133</v>
+      </c>
+      <c r="D22" s="19">
+        <v>90</v>
+      </c>
+      <c r="E22" s="21">
+        <v>107</v>
+      </c>
+      <c r="F22" s="23">
+        <v>122</v>
+      </c>
+      <c r="G22" s="19">
+        <v>93</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>637</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" thickBot="1">
+      <c r="A23">
+        <v>1942</v>
+      </c>
+      <c r="B23" s="24">
+        <v>84</v>
+      </c>
+      <c r="C23" s="16">
+        <v>23</v>
+      </c>
+      <c r="D23" s="18">
+        <v>53</v>
+      </c>
+      <c r="E23" s="12">
+        <v>41</v>
+      </c>
+      <c r="F23" s="13">
+        <v>64</v>
+      </c>
+      <c r="G23" s="11">
+        <v>25</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" thickBot="1">
+      <c r="A24">
+        <v>1943</v>
+      </c>
+      <c r="B24" s="23">
+        <v>122</v>
+      </c>
+      <c r="C24" s="13">
+        <v>61</v>
+      </c>
+      <c r="D24" s="16">
+        <v>24</v>
+      </c>
+      <c r="E24" s="18">
+        <v>54</v>
+      </c>
+      <c r="F24" s="17">
+        <v>7</v>
+      </c>
+      <c r="G24" s="18">
+        <v>50</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1">
+      <c r="A25">
+        <v>1944</v>
+      </c>
+      <c r="B25" s="11">
+        <v>26</v>
+      </c>
+      <c r="C25" s="11">
+        <v>33</v>
+      </c>
+      <c r="D25" s="17">
+        <v>11</v>
+      </c>
+      <c r="E25" s="19">
+        <v>85</v>
+      </c>
+      <c r="F25" s="21">
+        <v>106</v>
+      </c>
+      <c r="G25" s="18">
+        <v>50</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1">
+      <c r="A26">
+        <v>1945</v>
+      </c>
+      <c r="B26" s="15">
+        <v>101</v>
+      </c>
+      <c r="C26" s="11">
+        <v>27</v>
+      </c>
+      <c r="D26" s="12">
+        <v>44</v>
+      </c>
+      <c r="E26" s="23">
+        <v>122</v>
+      </c>
+      <c r="F26" s="15">
+        <v>101</v>
+      </c>
+      <c r="G26" s="25">
+        <v>141</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>536</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1">
+      <c r="A27">
+        <v>1946</v>
+      </c>
+      <c r="B27" s="16">
+        <v>22</v>
+      </c>
+      <c r="C27" s="13">
+        <v>56</v>
+      </c>
+      <c r="D27" s="12">
+        <v>37</v>
+      </c>
+      <c r="E27" s="11">
+        <v>31</v>
+      </c>
+      <c r="F27" s="11">
+        <v>34</v>
+      </c>
+      <c r="G27" s="22">
+        <v>155</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" thickBot="1">
+      <c r="A28">
+        <v>1947</v>
+      </c>
+      <c r="B28" s="19">
+        <v>85</v>
+      </c>
+      <c r="C28" s="21">
+        <v>114</v>
+      </c>
+      <c r="D28" s="24">
+        <v>77</v>
+      </c>
+      <c r="E28" s="19">
+        <v>93</v>
+      </c>
+      <c r="F28" s="19">
+        <v>90</v>
+      </c>
+      <c r="G28" s="20">
+        <v>133</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>592</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1">
+      <c r="A29">
+        <v>1948</v>
+      </c>
+      <c r="B29" s="26">
+        <v>149</v>
+      </c>
+      <c r="C29" s="16">
+        <v>21</v>
+      </c>
+      <c r="D29" s="17">
+        <v>14</v>
+      </c>
+      <c r="E29" s="19">
+        <v>86</v>
+      </c>
+      <c r="F29" s="21">
+        <v>106</v>
+      </c>
+      <c r="G29" s="21">
+        <v>109</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" thickBot="1">
+      <c r="A30">
+        <v>1949</v>
+      </c>
+      <c r="B30" s="24">
+        <v>80</v>
+      </c>
+      <c r="C30" s="17">
+        <v>8</v>
+      </c>
+      <c r="D30" s="12">
+        <v>39</v>
+      </c>
+      <c r="E30" s="11">
+        <v>33</v>
+      </c>
+      <c r="F30" s="12">
+        <v>44</v>
+      </c>
+      <c r="G30" s="18">
+        <v>52</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1">
+      <c r="A31">
+        <v>1950</v>
+      </c>
+      <c r="B31" s="16">
+        <v>25</v>
+      </c>
+      <c r="C31" s="20">
+        <v>129</v>
+      </c>
+      <c r="D31" s="12">
+        <v>41</v>
+      </c>
+      <c r="E31" s="10">
+        <v>75</v>
+      </c>
+      <c r="F31" s="31">
+        <v>211</v>
+      </c>
+      <c r="G31" s="19">
+        <v>86</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>567</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" thickBot="1">
+      <c r="A32">
+        <v>1951</v>
+      </c>
+      <c r="B32" s="25">
+        <v>145</v>
+      </c>
+      <c r="C32" s="27">
+        <v>169</v>
+      </c>
+      <c r="D32" s="24">
+        <v>83</v>
+      </c>
+      <c r="E32" s="12">
+        <v>43</v>
+      </c>
+      <c r="F32" s="27">
+        <v>169</v>
+      </c>
+      <c r="G32" s="25">
+        <v>138</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>747</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1">
+      <c r="A33">
+        <v>1952</v>
+      </c>
+      <c r="B33" s="22">
+        <v>156</v>
+      </c>
+      <c r="C33" s="19">
+        <v>93</v>
+      </c>
+      <c r="D33" s="10">
+        <v>74</v>
+      </c>
+      <c r="E33" s="12">
+        <v>43</v>
+      </c>
+      <c r="F33" s="15">
+        <v>104</v>
+      </c>
+      <c r="G33" s="15">
+        <v>96</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>566</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1">
+      <c r="A34">
+        <v>1953</v>
+      </c>
+      <c r="B34" s="16">
+        <v>18</v>
+      </c>
+      <c r="C34" s="18">
+        <v>50</v>
+      </c>
+      <c r="D34" s="17">
+        <v>11</v>
+      </c>
+      <c r="E34" s="26">
+        <v>154</v>
+      </c>
+      <c r="F34" s="29">
+        <v>176</v>
+      </c>
+      <c r="G34" s="32">
+        <v>244</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>653</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1">
+      <c r="A35">
+        <v>1954</v>
+      </c>
+      <c r="B35" s="13">
+        <v>64</v>
+      </c>
+      <c r="C35" s="20">
+        <v>125</v>
+      </c>
+      <c r="D35" s="21">
+        <v>109</v>
+      </c>
+      <c r="E35" s="10">
+        <v>74</v>
+      </c>
+      <c r="F35" s="11">
+        <v>30</v>
+      </c>
+      <c r="G35" s="17">
+        <v>12</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" thickBot="1">
+      <c r="A36">
+        <v>1955</v>
+      </c>
+      <c r="B36" s="22">
+        <v>161</v>
+      </c>
+      <c r="C36" s="21">
+        <v>110</v>
+      </c>
+      <c r="D36" s="17">
+        <v>14</v>
+      </c>
+      <c r="E36" s="13">
+        <v>63</v>
+      </c>
+      <c r="F36" s="24">
+        <v>78</v>
+      </c>
+      <c r="G36" s="24">
+        <v>79</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1">
+      <c r="A37">
+        <v>1956</v>
+      </c>
+      <c r="B37" s="19">
+        <v>90</v>
+      </c>
+      <c r="C37" s="12">
+        <v>38</v>
+      </c>
+      <c r="D37" s="11">
+        <v>33</v>
+      </c>
+      <c r="E37" s="13">
+        <v>63</v>
+      </c>
+      <c r="F37" s="18">
+        <v>48</v>
+      </c>
+      <c r="G37" s="23">
+        <v>125</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1">
+      <c r="A38">
+        <v>1957</v>
+      </c>
+      <c r="B38" s="12">
+        <v>42</v>
+      </c>
+      <c r="C38" s="26">
+        <v>149</v>
+      </c>
+      <c r="D38" s="13">
+        <v>58</v>
+      </c>
+      <c r="E38" s="11">
+        <v>28</v>
+      </c>
+      <c r="F38" s="13">
+        <v>58</v>
+      </c>
+      <c r="G38" s="13">
+        <v>56</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1">
+      <c r="A39">
+        <v>1958</v>
+      </c>
+      <c r="B39" s="29">
+        <v>183</v>
+      </c>
+      <c r="C39" s="12">
+        <v>36</v>
+      </c>
+      <c r="D39" s="25">
+        <v>144</v>
+      </c>
+      <c r="E39" s="11">
+        <v>30</v>
+      </c>
+      <c r="F39" s="18">
+        <v>55</v>
+      </c>
+      <c r="G39" s="19">
+        <v>92</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" thickBot="1">
+      <c r="A40">
+        <v>1959</v>
+      </c>
+      <c r="B40" s="24">
+        <v>82</v>
+      </c>
+      <c r="C40" s="17">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="15" thickBot="1">
-      <c r="A2" s="7">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15" thickBot="1">
-      <c r="A3" s="3">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15" thickBot="1">
-      <c r="A4" s="37">
-        <v>999.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15" thickBot="1">
-      <c r="A5" s="4">
-        <v>14.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15" thickBot="1">
-      <c r="A6" s="4">
+      <c r="D40" s="13">
+        <v>62</v>
+      </c>
+      <c r="E40" s="11">
+        <v>33</v>
+      </c>
+      <c r="F40" s="12">
+        <v>41</v>
+      </c>
+      <c r="G40" s="26">
+        <v>150</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" thickBot="1">
+      <c r="A41">
+        <v>1960</v>
+      </c>
+      <c r="B41" s="10">
+        <v>72</v>
+      </c>
+      <c r="C41" s="15">
+        <v>101</v>
+      </c>
+      <c r="D41" s="24">
+        <v>82</v>
+      </c>
+      <c r="E41" s="26">
+        <v>149</v>
+      </c>
+      <c r="F41" s="19">
+        <v>90</v>
+      </c>
+      <c r="G41" s="32">
+        <v>254</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>748</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" thickBot="1">
+      <c r="A42">
+        <v>1961</v>
+      </c>
+      <c r="B42" s="22">
+        <v>156</v>
+      </c>
+      <c r="C42" s="18">
+        <v>48</v>
+      </c>
+      <c r="D42" s="14">
+        <v>0</v>
+      </c>
+      <c r="E42" s="34">
+        <v>226</v>
+      </c>
+      <c r="F42" s="27">
+        <v>171</v>
+      </c>
+      <c r="G42" s="26">
+        <v>147</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>748</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" thickBot="1">
+      <c r="A43">
+        <v>1962</v>
+      </c>
+      <c r="B43" s="23">
+        <v>125</v>
+      </c>
+      <c r="C43" s="12">
+        <v>37</v>
+      </c>
+      <c r="D43" s="15">
+        <v>100</v>
+      </c>
+      <c r="E43" s="23">
+        <v>116</v>
+      </c>
+      <c r="F43" s="25">
+        <v>137</v>
+      </c>
+      <c r="G43" s="23">
+        <v>125</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" thickBot="1">
+      <c r="A44">
+        <v>1963</v>
+      </c>
+      <c r="B44" s="13">
+        <v>57</v>
+      </c>
+      <c r="C44" s="15">
+        <v>104</v>
+      </c>
+      <c r="D44" s="20">
+        <v>129</v>
+      </c>
+      <c r="E44" s="19">
+        <v>91</v>
+      </c>
+      <c r="F44" s="24">
+        <v>84</v>
+      </c>
+      <c r="G44" s="15">
+        <v>101</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>566</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" thickBot="1">
+      <c r="A45">
+        <v>1964</v>
+      </c>
+      <c r="B45" s="17">
+        <v>10</v>
+      </c>
+      <c r="C45" s="13">
+        <v>55</v>
+      </c>
+      <c r="D45" s="13">
+        <v>64</v>
+      </c>
+      <c r="E45" s="18">
+        <v>48</v>
+      </c>
+      <c r="F45" s="21">
+        <v>115</v>
+      </c>
+      <c r="G45" s="11">
+        <v>35</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15" thickBot="1">
+      <c r="A46">
+        <v>1965</v>
+      </c>
+      <c r="B46" s="20">
+        <v>128</v>
+      </c>
+      <c r="C46" s="17">
+        <v>12</v>
+      </c>
+      <c r="D46" s="19">
+        <v>90</v>
+      </c>
+      <c r="E46" s="30">
+        <v>194</v>
+      </c>
+      <c r="F46" s="18">
+        <v>48</v>
+      </c>
+      <c r="G46" s="24">
+        <v>77</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>549</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15" thickBot="1">
+      <c r="A47">
+        <v>1966</v>
+      </c>
+      <c r="B47" s="25">
+        <v>144</v>
+      </c>
+      <c r="C47" s="23">
+        <v>119</v>
+      </c>
+      <c r="D47" s="12">
+        <v>41</v>
+      </c>
+      <c r="E47" s="16">
+        <v>22</v>
+      </c>
+      <c r="F47" s="31">
+        <v>212</v>
+      </c>
+      <c r="G47" s="28">
+        <v>197</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="0"/>
+        <v>735</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15" thickBot="1">
+      <c r="A48">
+        <v>1967</v>
+      </c>
+      <c r="B48" s="18">
+        <v>49</v>
+      </c>
+      <c r="C48" s="19">
+        <v>89</v>
+      </c>
+      <c r="D48" s="18">
+        <v>50</v>
+      </c>
+      <c r="E48" s="25">
+        <v>142</v>
+      </c>
+      <c r="F48" s="25">
+        <v>139</v>
+      </c>
+      <c r="G48" s="29">
+        <v>178</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="0"/>
+        <v>647</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15" thickBot="1">
+      <c r="A49">
+        <v>1968</v>
+      </c>
+      <c r="B49" s="15">
+        <v>98</v>
+      </c>
+      <c r="C49" s="15">
+        <v>102</v>
+      </c>
+      <c r="D49" s="12">
+        <v>37</v>
+      </c>
+      <c r="E49" s="23">
+        <v>115</v>
+      </c>
+      <c r="F49" s="19">
+        <v>93</v>
+      </c>
+      <c r="G49" s="13">
+        <v>64</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="0"/>
+        <v>509</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" thickBot="1">
+      <c r="A50">
+        <v>1969</v>
+      </c>
+      <c r="B50" s="20">
+        <v>132</v>
+      </c>
+      <c r="C50" s="13">
+        <v>63</v>
+      </c>
+      <c r="D50" s="19">
+        <v>91</v>
+      </c>
+      <c r="E50" s="12">
+        <v>38</v>
+      </c>
+      <c r="F50" s="16">
+        <v>21</v>
+      </c>
+      <c r="G50" s="25">
+        <v>136</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="0"/>
+        <v>481</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15" thickBot="1">
+      <c r="A51">
+        <v>1970</v>
+      </c>
+      <c r="B51" s="24">
+        <v>80</v>
+      </c>
+      <c r="C51" s="22">
+        <v>160</v>
+      </c>
+      <c r="D51" s="18">
+        <v>55</v>
+      </c>
+      <c r="E51" s="17">
+        <v>11</v>
+      </c>
+      <c r="F51" s="26">
+        <v>145</v>
+      </c>
+      <c r="G51" s="21">
+        <v>112</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15" thickBot="1">
+      <c r="A52">
+        <v>1971</v>
+      </c>
+      <c r="B52" s="20">
+        <v>127</v>
+      </c>
+      <c r="C52" s="24">
+        <v>83</v>
+      </c>
+      <c r="D52" s="18">
+        <v>52</v>
+      </c>
+      <c r="E52" s="12">
+        <v>35</v>
+      </c>
+      <c r="F52" s="25">
+        <v>137</v>
+      </c>
+      <c r="G52" s="18">
+        <v>54</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="0"/>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15" thickBot="1">
+      <c r="A53">
+        <v>1972</v>
+      </c>
+      <c r="B53" s="19">
+        <v>89</v>
+      </c>
+      <c r="C53" s="21">
+        <v>111</v>
+      </c>
+      <c r="D53" s="10">
+        <v>72</v>
+      </c>
+      <c r="E53" s="11">
+        <v>31</v>
+      </c>
+      <c r="F53" s="21">
+        <v>113</v>
+      </c>
+      <c r="G53" s="18">
+        <v>50</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="0"/>
+        <v>466</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15" thickBot="1">
+      <c r="A54">
+        <v>1973</v>
+      </c>
+      <c r="B54" s="13">
+        <v>62</v>
+      </c>
+      <c r="C54" s="23">
+        <v>117</v>
+      </c>
+      <c r="D54" s="16">
+        <v>21</v>
+      </c>
+      <c r="E54" s="12">
+        <v>36</v>
+      </c>
+      <c r="F54" s="10">
+        <v>73</v>
+      </c>
+      <c r="G54" s="18">
+        <v>47</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="0"/>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15" thickBot="1">
+      <c r="A55">
+        <v>1974</v>
+      </c>
+      <c r="B55" s="13">
+        <v>65</v>
+      </c>
+      <c r="C55" s="20">
+        <v>132</v>
+      </c>
+      <c r="D55" s="19">
+        <v>88</v>
+      </c>
+      <c r="E55" s="15">
+        <v>96</v>
+      </c>
+      <c r="F55" s="18">
+        <v>50</v>
+      </c>
+      <c r="G55" s="10">
+        <v>73</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="0"/>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15" thickBot="1">
+      <c r="A56">
+        <v>1975</v>
+      </c>
+      <c r="B56" s="19">
+        <v>90</v>
+      </c>
+      <c r="C56" s="11">
+        <v>34</v>
+      </c>
+      <c r="D56" s="15">
+        <v>99</v>
+      </c>
+      <c r="E56" s="25">
+        <v>137</v>
+      </c>
+      <c r="F56" s="21">
+        <v>111</v>
+      </c>
+      <c r="G56" s="11">
+        <v>31</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="0"/>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15" thickBot="1">
+      <c r="A57">
+        <v>1976</v>
+      </c>
+      <c r="B57" s="11">
+        <v>25</v>
+      </c>
+      <c r="C57" s="10">
+        <v>68</v>
+      </c>
+      <c r="D57" s="13">
+        <v>55</v>
+      </c>
+      <c r="E57" s="12">
+        <v>41</v>
+      </c>
+      <c r="F57" s="26">
+        <v>152</v>
+      </c>
+      <c r="G57" s="12">
+        <v>39</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15" thickBot="1">
+      <c r="A58">
+        <v>1977</v>
+      </c>
+      <c r="B58" s="15">
+        <v>95</v>
+      </c>
+      <c r="C58" s="26">
+        <v>146</v>
+      </c>
+      <c r="D58" s="10">
+        <v>71</v>
+      </c>
+      <c r="E58" s="29">
+        <v>175</v>
+      </c>
+      <c r="F58" s="26">
+        <v>154</v>
+      </c>
+      <c r="G58" s="21">
+        <v>114</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="0"/>
+        <v>755</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15" thickBot="1">
+      <c r="A59">
+        <v>1978</v>
+      </c>
+      <c r="B59" s="29">
+        <v>179</v>
+      </c>
+      <c r="C59" s="24">
+        <v>83</v>
+      </c>
+      <c r="D59" s="25">
+        <v>145</v>
+      </c>
+      <c r="E59" s="13">
+        <v>61</v>
+      </c>
+      <c r="F59" s="10">
+        <v>72</v>
+      </c>
+      <c r="G59" s="24">
+        <v>82</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="0"/>
+        <v>622</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15" thickBot="1">
+      <c r="A60">
+        <v>1979</v>
+      </c>
+      <c r="B60" s="26">
+        <v>150</v>
+      </c>
+      <c r="C60" s="21">
+        <v>112</v>
+      </c>
+      <c r="D60" s="30">
+        <v>190</v>
+      </c>
+      <c r="E60" s="17">
+        <v>6</v>
+      </c>
+      <c r="F60" s="17">
+        <v>10</v>
+      </c>
+      <c r="G60" s="20">
+        <v>134</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="0"/>
+        <v>602</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15" thickBot="1">
+      <c r="A61">
+        <v>1980</v>
+      </c>
+      <c r="B61" s="23">
+        <v>121</v>
+      </c>
+      <c r="C61" s="11">
+        <v>26</v>
+      </c>
+      <c r="D61" s="15">
+        <v>97</v>
+      </c>
+      <c r="E61" s="13">
+        <v>59</v>
+      </c>
+      <c r="F61" s="21">
+        <v>111</v>
+      </c>
+      <c r="G61" s="25">
+        <v>138</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="0"/>
+        <v>552</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15" thickBot="1">
+      <c r="A62">
+        <v>1981</v>
+      </c>
+      <c r="B62" s="24">
+        <v>82</v>
+      </c>
+      <c r="C62" s="18">
+        <v>54</v>
+      </c>
+      <c r="D62" s="24">
+        <v>83</v>
+      </c>
+      <c r="E62" s="22">
+        <v>160</v>
+      </c>
+      <c r="F62" s="12">
+        <v>43</v>
+      </c>
+      <c r="G62" s="24">
+        <v>76</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="0"/>
+        <v>498</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15" thickBot="1">
+      <c r="A63">
+        <v>1982</v>
+      </c>
+      <c r="B63" s="15">
+        <v>103</v>
+      </c>
+      <c r="C63" s="18">
+        <v>53</v>
+      </c>
+      <c r="D63" s="19">
+        <v>92</v>
+      </c>
+      <c r="E63" s="20">
+        <v>134</v>
+      </c>
+      <c r="F63" s="16">
+        <v>21</v>
+      </c>
+      <c r="G63" s="32">
+        <v>306</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="0"/>
+        <v>709</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15" thickBot="1">
+      <c r="A64">
+        <v>1983</v>
+      </c>
+      <c r="B64" s="11">
+        <v>27</v>
+      </c>
+      <c r="C64" s="19">
+        <v>93</v>
+      </c>
+      <c r="D64" s="10">
+        <v>71</v>
+      </c>
+      <c r="E64" s="31">
+        <v>211</v>
+      </c>
+      <c r="F64" s="21">
+        <v>106</v>
+      </c>
+      <c r="G64" s="30">
+        <v>191</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="0"/>
+        <v>699</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15" thickBot="1">
+      <c r="A65">
+        <v>1984</v>
+      </c>
+      <c r="B65" s="30">
+        <v>191</v>
+      </c>
+      <c r="C65" s="19">
+        <v>92</v>
+      </c>
+      <c r="D65" s="19">
+        <v>91</v>
+      </c>
+      <c r="E65" s="11">
+        <v>28</v>
+      </c>
+      <c r="F65" s="12">
+        <v>38</v>
+      </c>
+      <c r="G65" s="20">
+        <v>133</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="0"/>
+        <v>573</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15" thickBot="1">
+      <c r="A66">
+        <v>1985</v>
+      </c>
+      <c r="B66" s="10">
+        <v>70</v>
+      </c>
+      <c r="C66" s="24">
+        <v>85</v>
+      </c>
+      <c r="D66" s="21">
+        <v>115</v>
+      </c>
+      <c r="E66" s="26">
+        <v>150</v>
+      </c>
+      <c r="F66" s="27">
+        <v>171</v>
+      </c>
+      <c r="G66" s="24">
+        <v>77</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="0"/>
+        <v>668</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15" thickBot="1">
+      <c r="A67">
+        <v>1986</v>
+      </c>
+      <c r="B67" s="28">
+        <v>203</v>
+      </c>
+      <c r="C67" s="24">
+        <v>76</v>
+      </c>
+      <c r="D67" s="18">
+        <v>51</v>
+      </c>
+      <c r="E67" s="17">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" ht="15" thickBot="1">
-      <c r="A7" s="4">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15" thickBot="1">
-      <c r="A8" s="3">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="15" thickBot="1">
-      <c r="A9" s="4">
-        <v>14.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15" thickBot="1">
-      <c r="A10" s="3">
+      <c r="F67" s="10">
+        <v>72</v>
+      </c>
+      <c r="G67" s="15">
+        <v>103</v>
+      </c>
+      <c r="H67">
+        <f t="shared" ref="H67:H102" si="1">SUM(B67:D67)+SUM(E67:G67)</f>
+        <v>519</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15" thickBot="1">
+      <c r="A68">
+        <v>1987</v>
+      </c>
+      <c r="B68" s="11">
+        <v>29</v>
+      </c>
+      <c r="C68" s="18">
+        <v>54</v>
+      </c>
+      <c r="D68" s="24">
+        <v>76</v>
+      </c>
+      <c r="E68" s="10">
+        <v>75</v>
+      </c>
+      <c r="F68" s="18">
+        <v>50</v>
+      </c>
+      <c r="G68" s="21">
+        <v>114</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="1"/>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15" thickBot="1">
+      <c r="A69">
+        <v>1988</v>
+      </c>
+      <c r="B69" s="34">
+        <v>225</v>
+      </c>
+      <c r="C69" s="21">
+        <v>111</v>
+      </c>
+      <c r="D69" s="23">
+        <v>122</v>
+      </c>
+      <c r="E69" s="25">
+        <v>142</v>
+      </c>
+      <c r="F69" s="15">
+        <v>101</v>
+      </c>
+      <c r="G69" s="11">
+        <v>34</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="1"/>
+        <v>735</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15" thickBot="1">
+      <c r="A70">
+        <v>1989</v>
+      </c>
+      <c r="B70" s="11">
+        <v>29</v>
+      </c>
+      <c r="C70" s="19">
+        <v>90</v>
+      </c>
+      <c r="D70" s="12">
+        <v>43</v>
+      </c>
+      <c r="E70" s="18">
+        <v>49</v>
+      </c>
+      <c r="F70" s="16">
+        <v>22</v>
+      </c>
+      <c r="G70" s="18">
+        <v>50</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="1"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15" thickBot="1">
+      <c r="A71">
+        <v>1990</v>
+      </c>
+      <c r="B71" s="10">
+        <v>73</v>
+      </c>
+      <c r="C71" s="22">
+        <v>155</v>
+      </c>
+      <c r="D71" s="14">
+        <v>4</v>
+      </c>
+      <c r="E71" s="11">
+        <v>33</v>
+      </c>
+      <c r="F71" s="24">
+        <v>81</v>
+      </c>
+      <c r="G71" s="11">
+        <v>34</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="1"/>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15" thickBot="1">
+      <c r="A72">
+        <v>1991</v>
+      </c>
+      <c r="B72" s="12">
+        <v>42</v>
+      </c>
+      <c r="C72" s="13">
+        <v>56</v>
+      </c>
+      <c r="D72" s="12">
+        <v>40</v>
+      </c>
+      <c r="E72" s="29">
+        <v>178</v>
+      </c>
+      <c r="F72" s="26">
+        <v>145</v>
+      </c>
+      <c r="G72" s="13">
+        <v>58</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="1"/>
+        <v>519</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15" thickBot="1">
+      <c r="A73">
+        <v>1992</v>
+      </c>
+      <c r="B73" s="11">
+        <v>25</v>
+      </c>
+      <c r="C73" s="16">
+        <v>16</v>
+      </c>
+      <c r="D73" s="24">
+        <v>79</v>
+      </c>
+      <c r="E73" s="25">
+        <v>145</v>
+      </c>
+      <c r="F73" s="30">
+        <v>185</v>
+      </c>
+      <c r="G73" s="12">
+        <v>38</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="1"/>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15" thickBot="1">
+      <c r="A74">
+        <v>1993</v>
+      </c>
+      <c r="B74" s="17">
+        <v>14</v>
+      </c>
+      <c r="C74" s="14">
+        <v>3</v>
+      </c>
+      <c r="D74" s="17">
+        <v>15</v>
+      </c>
+      <c r="E74" s="26">
+        <v>145</v>
+      </c>
+      <c r="F74" s="26">
+        <v>152</v>
+      </c>
+      <c r="G74" s="23">
+        <v>117</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="1"/>
+        <v>446</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15" thickBot="1">
+      <c r="A75">
+        <v>1994</v>
+      </c>
+      <c r="B75" s="29">
+        <v>176</v>
+      </c>
+      <c r="C75" s="21">
+        <v>109</v>
+      </c>
+      <c r="D75" s="16">
+        <v>18</v>
+      </c>
+      <c r="E75" s="20">
+        <v>129</v>
+      </c>
+      <c r="F75" s="18">
+        <v>46</v>
+      </c>
+      <c r="G75" s="34">
+        <v>231</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="1"/>
+        <v>709</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15" thickBot="1">
+      <c r="A76">
+        <v>1995</v>
+      </c>
+      <c r="B76" s="20">
+        <v>135</v>
+      </c>
+      <c r="C76" s="21">
+        <v>111</v>
+      </c>
+      <c r="D76" s="24">
+        <v>81</v>
+      </c>
+      <c r="E76" s="13">
+        <v>61</v>
+      </c>
+      <c r="F76" s="24">
+        <v>78</v>
+      </c>
+      <c r="G76" s="15">
+        <v>102</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="1"/>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15" thickBot="1">
+      <c r="A77">
+        <v>1996</v>
+      </c>
+      <c r="B77" s="15">
+        <v>97</v>
+      </c>
+      <c r="C77" s="21">
+        <v>114</v>
+      </c>
+      <c r="D77" s="18">
+        <v>52</v>
+      </c>
+      <c r="E77" s="13">
+        <v>56</v>
+      </c>
+      <c r="F77" s="24">
+        <v>84</v>
+      </c>
+      <c r="G77" s="34">
+        <v>233</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="1"/>
+        <v>636</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15" thickBot="1">
+      <c r="A78">
+        <v>1997</v>
+      </c>
+      <c r="B78" s="12">
+        <v>43</v>
+      </c>
+      <c r="C78" s="10">
+        <v>73</v>
+      </c>
+      <c r="D78" s="16">
+        <v>15</v>
+      </c>
+      <c r="E78" s="13">
+        <v>61</v>
+      </c>
+      <c r="F78" s="31">
+        <v>209</v>
+      </c>
+      <c r="G78" s="13">
+        <v>59</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="1"/>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15" thickBot="1">
+      <c r="A79">
+        <v>1998</v>
+      </c>
+      <c r="B79" s="21">
+        <v>108</v>
+      </c>
+      <c r="C79" s="11">
+        <v>26</v>
+      </c>
+      <c r="D79" s="13">
+        <v>56</v>
+      </c>
+      <c r="E79" s="12">
+        <v>35</v>
+      </c>
+      <c r="F79" s="32">
+        <v>268</v>
+      </c>
+      <c r="G79" s="28">
+        <v>200</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="1"/>
+        <v>693</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15" thickBot="1">
+      <c r="A80">
+        <v>1999</v>
+      </c>
+      <c r="B80" s="10">
+        <v>69</v>
+      </c>
+      <c r="C80" s="19">
+        <v>92</v>
+      </c>
+      <c r="D80" s="13">
+        <v>56</v>
+      </c>
+      <c r="E80" s="23">
+        <v>115</v>
+      </c>
+      <c r="F80" s="21">
+        <v>110</v>
+      </c>
+      <c r="G80" s="13">
+        <v>59</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="1"/>
+        <v>501</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15" thickBot="1">
+      <c r="A81">
+        <v>2000</v>
+      </c>
+      <c r="B81" s="16">
+        <v>17</v>
+      </c>
+      <c r="C81" s="15">
+        <v>104</v>
+      </c>
+      <c r="D81" s="18">
+        <v>52</v>
+      </c>
+      <c r="E81" s="15">
+        <v>96</v>
+      </c>
+      <c r="F81" s="13">
+        <v>58</v>
+      </c>
+      <c r="G81" s="22">
+        <v>161</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="1"/>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15" thickBot="1">
+      <c r="A82">
+        <v>2001</v>
+      </c>
+      <c r="B82" s="20">
+        <v>134</v>
+      </c>
+      <c r="C82" s="13">
+        <v>58</v>
+      </c>
+      <c r="D82" s="20">
+        <v>134</v>
+      </c>
+      <c r="E82" s="22">
+        <v>159</v>
+      </c>
+      <c r="F82" s="32">
+        <v>322</v>
+      </c>
+      <c r="G82" s="23">
+        <v>119</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="1"/>
+        <v>926</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15" thickBot="1">
+      <c r="A83">
+        <v>2002</v>
+      </c>
+      <c r="B83" s="16">
+        <v>22</v>
+      </c>
+      <c r="C83" s="18">
+        <v>54</v>
+      </c>
+      <c r="D83" s="11">
+        <v>29</v>
+      </c>
+      <c r="E83" s="24">
+        <v>82</v>
+      </c>
+      <c r="F83" s="18">
+        <v>47</v>
+      </c>
+      <c r="G83" s="12">
+        <v>43</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="15" thickBot="1">
+      <c r="A84">
+        <v>2003</v>
+      </c>
+      <c r="B84" s="19">
+        <v>93</v>
+      </c>
+      <c r="C84" s="13">
+        <v>57</v>
+      </c>
+      <c r="D84" s="11">
+        <v>29</v>
+      </c>
+      <c r="E84" s="10">
+        <v>74</v>
+      </c>
+      <c r="F84" s="23">
+        <v>117</v>
+      </c>
+      <c r="G84" s="19">
+        <v>91</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="1"/>
+        <v>461</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15" thickBot="1">
+      <c r="A85">
+        <v>2004</v>
+      </c>
+      <c r="B85" s="25">
+        <v>136</v>
+      </c>
+      <c r="C85" s="16">
+        <v>20</v>
+      </c>
+      <c r="D85" s="12">
+        <v>38</v>
+      </c>
+      <c r="E85" s="22">
+        <v>155</v>
+      </c>
+      <c r="F85" s="10">
+        <v>70</v>
+      </c>
+      <c r="G85" s="10">
+        <v>68</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="1"/>
+        <v>487</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15" thickBot="1">
+      <c r="A86">
+        <v>2005</v>
+      </c>
+      <c r="B86" s="11">
+        <v>32</v>
+      </c>
+      <c r="C86" s="12">
+        <v>38</v>
+      </c>
+      <c r="D86" s="12">
+        <v>38</v>
+      </c>
+      <c r="E86" s="15">
+        <v>97</v>
+      </c>
+      <c r="F86" s="17">
+        <v>11</v>
+      </c>
+      <c r="G86" s="10">
+        <v>68</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="1"/>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15" thickBot="1">
+      <c r="A87">
+        <v>2006</v>
+      </c>
+      <c r="B87" s="18">
+        <v>49</v>
+      </c>
+      <c r="C87" s="15">
+        <v>100</v>
+      </c>
+      <c r="D87" s="30">
+        <v>185</v>
+      </c>
+      <c r="E87" s="13">
+        <v>55</v>
+      </c>
+      <c r="F87" s="19">
+        <v>90</v>
+      </c>
+      <c r="G87" s="21">
+        <v>112</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="1"/>
+        <v>591</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15" thickBot="1">
+      <c r="A88">
+        <v>2007</v>
+      </c>
+      <c r="B88" s="24">
+        <v>82</v>
+      </c>
+      <c r="C88" s="25">
+        <v>139</v>
+      </c>
+      <c r="D88" s="19">
+        <v>93</v>
+      </c>
+      <c r="E88" s="13">
+        <v>55</v>
+      </c>
+      <c r="F88" s="10">
+        <v>68</v>
+      </c>
+      <c r="G88" s="18">
+        <v>49</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="1"/>
+        <v>486</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15" thickBot="1">
+      <c r="A89">
+        <v>2008</v>
+      </c>
+      <c r="B89" s="21">
+        <v>108</v>
+      </c>
+      <c r="C89" s="11">
+        <v>31</v>
+      </c>
+      <c r="D89" s="15">
+        <v>102</v>
+      </c>
+      <c r="E89" s="18">
+        <v>48</v>
+      </c>
+      <c r="F89" s="12">
+        <v>35</v>
+      </c>
+      <c r="G89" s="24">
+        <v>75</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="1"/>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15" thickBot="1">
+      <c r="A90">
+        <v>2009</v>
+      </c>
+      <c r="B90" s="20">
+        <v>129</v>
+      </c>
+      <c r="C90" s="11">
+        <v>33</v>
+      </c>
+      <c r="D90" s="11">
+        <v>31</v>
+      </c>
+      <c r="E90" s="19">
+        <v>90</v>
+      </c>
+      <c r="F90" s="20">
+        <v>131</v>
+      </c>
+      <c r="G90" s="10">
+        <v>74</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="1"/>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15" thickBot="1">
+      <c r="A91">
+        <v>2010</v>
+      </c>
+      <c r="B91" s="24">
+        <v>78</v>
+      </c>
+      <c r="C91" s="18">
+        <v>54</v>
+      </c>
+      <c r="D91" s="10">
+        <v>68</v>
+      </c>
+      <c r="E91" s="11">
+        <v>34</v>
+      </c>
+      <c r="F91" s="28">
+        <v>204</v>
+      </c>
+      <c r="G91" s="19">
+        <v>92</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="1"/>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15" thickBot="1">
+      <c r="A92">
+        <v>2011</v>
+      </c>
+      <c r="B92" s="11">
+        <v>27</v>
+      </c>
+      <c r="C92" s="13">
+        <v>62</v>
+      </c>
+      <c r="D92" s="11">
+        <v>34</v>
+      </c>
+      <c r="E92" s="19">
+        <v>93</v>
+      </c>
+      <c r="F92" s="33">
+        <v>215</v>
+      </c>
+      <c r="G92" s="24">
+        <v>80</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="1"/>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="15" thickBot="1">
+      <c r="A93">
+        <v>2012</v>
+      </c>
+      <c r="B93" s="18">
+        <v>53</v>
+      </c>
+      <c r="C93" s="17">
+        <v>6</v>
+      </c>
+      <c r="D93" s="11">
+        <v>31</v>
+      </c>
+      <c r="E93" s="12">
+        <v>40</v>
+      </c>
+      <c r="F93" s="12">
+        <v>36</v>
+      </c>
+      <c r="G93" s="29">
+        <v>175</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="1"/>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="15" thickBot="1">
+      <c r="A94">
+        <v>2013</v>
+      </c>
+      <c r="B94" s="25">
+        <v>138</v>
+      </c>
+      <c r="C94" s="24">
+        <v>77</v>
+      </c>
+      <c r="D94" s="10">
+        <v>71</v>
+      </c>
+      <c r="E94" s="23">
+        <v>116</v>
+      </c>
+      <c r="F94" s="10">
+        <v>74</v>
+      </c>
+      <c r="G94" s="27">
+        <v>170</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="1"/>
+        <v>646</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15" thickBot="1">
+      <c r="A95">
+        <v>2014</v>
+      </c>
+      <c r="B95" s="29">
+        <v>184</v>
+      </c>
+      <c r="C95" s="20">
+        <v>130</v>
+      </c>
+      <c r="D95" s="19">
+        <v>88</v>
+      </c>
+      <c r="E95" s="19">
+        <v>87</v>
+      </c>
+      <c r="F95" s="23">
+        <v>116</v>
+      </c>
+      <c r="G95" s="10">
+        <v>69</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="1"/>
+        <v>674</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="15" thickBot="1">
+      <c r="A96">
+        <v>2015</v>
+      </c>
+      <c r="B96" s="19">
+        <v>94</v>
+      </c>
+      <c r="C96" s="24">
+        <v>80</v>
+      </c>
+      <c r="D96" s="12">
+        <v>40</v>
+      </c>
+      <c r="E96" s="12">
+        <v>41</v>
+      </c>
+      <c r="F96" s="20">
+        <v>130</v>
+      </c>
+      <c r="G96" s="18">
+        <v>54</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="1"/>
+        <v>439</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="15" thickBot="1">
+      <c r="A97">
+        <v>2016</v>
+      </c>
+      <c r="B97" s="34">
+        <v>234</v>
+      </c>
+      <c r="C97" s="26">
+        <v>152</v>
+      </c>
+      <c r="D97" s="21">
+        <v>110</v>
+      </c>
+      <c r="E97" s="18">
+        <v>52</v>
+      </c>
+      <c r="F97" s="18">
+        <v>52</v>
+      </c>
+      <c r="G97" s="17">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" ht="15" thickBot="1">
-      <c r="A11" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="15" thickBot="1">
-      <c r="A12" s="3">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15" thickBot="1">
-      <c r="A13" s="3">
-        <v>12.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="15" thickBot="1">
-      <c r="A14" s="4">
-        <v>14.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="15" thickBot="1">
-      <c r="A15" s="4">
-        <v>13.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="15" thickBot="1">
-      <c r="A16" s="3">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15" thickBot="1">
-      <c r="A17" s="2">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="15" thickBot="1">
-      <c r="A18" s="3">
-        <v>12.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="15" thickBot="1">
-      <c r="A19" s="3">
-        <v>13.4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15" thickBot="1">
-      <c r="A20" s="3">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="15" thickBot="1">
-      <c r="A21" s="37">
-        <v>999.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="15" thickBot="1">
-      <c r="A22" s="37">
-        <v>999.9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="15" thickBot="1">
-      <c r="A23" s="37">
-        <v>999.9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="15" thickBot="1">
-      <c r="A24" s="37">
-        <v>999.9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="15" thickBot="1">
-      <c r="A25" s="37">
-        <v>999.9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="15" thickBot="1">
-      <c r="A26" s="4">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="15" thickBot="1">
-      <c r="A27" s="4">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="15" thickBot="1">
-      <c r="A28" s="4">
-        <v>13.9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="15" thickBot="1">
-      <c r="A29" s="3">
-        <v>12.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="15" thickBot="1">
-      <c r="A30" s="4">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="15" thickBot="1">
-      <c r="A31" s="4">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="15" thickBot="1">
-      <c r="A32" s="3">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="15" thickBot="1">
-      <c r="A33" s="4">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="15" thickBot="1">
-      <c r="A34" s="3">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="15" thickBot="1">
-      <c r="A35" s="4">
+      <c r="H97">
+        <f t="shared" si="1"/>
+        <v>613</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="15" thickBot="1">
+      <c r="A98">
+        <v>2017</v>
+      </c>
+      <c r="B98" s="11">
+        <v>28</v>
+      </c>
+      <c r="C98" s="24">
+        <v>75</v>
+      </c>
+      <c r="D98" s="10">
+        <v>65</v>
+      </c>
+      <c r="E98" s="17">
+        <v>12</v>
+      </c>
+      <c r="F98" s="19">
+        <v>86</v>
+      </c>
+      <c r="G98" s="17">
+        <v>13</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="1"/>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="15" thickBot="1">
+      <c r="A99">
+        <v>2018</v>
+      </c>
+      <c r="B99" s="23">
+        <v>122</v>
+      </c>
+      <c r="C99" s="18">
+        <v>50</v>
+      </c>
+      <c r="D99" s="21">
+        <v>113</v>
+      </c>
+      <c r="E99" s="17">
+        <v>13</v>
+      </c>
+      <c r="F99" s="10">
+        <v>65</v>
+      </c>
+      <c r="G99" s="22">
+        <v>163</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="1"/>
+        <v>526</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="15" thickBot="1">
+      <c r="A100">
+        <v>2019</v>
+      </c>
+      <c r="B100" s="17">
+        <v>6</v>
+      </c>
+      <c r="C100" s="17">
+        <v>6</v>
+      </c>
+      <c r="D100" s="17">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" ht="15" thickBot="1">
-      <c r="A36" s="3">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="15" thickBot="1">
-      <c r="A37" s="3">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="15" thickBot="1">
-      <c r="A38" s="3">
-        <v>12.9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="15" thickBot="1">
-      <c r="A39" s="3">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="15" thickBot="1">
-      <c r="A40" s="3">
-        <v>13.3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="15" thickBot="1">
-      <c r="A41" s="3">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="15" thickBot="1">
-      <c r="A42" s="4">
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="15" thickBot="1">
-      <c r="A43" s="3">
-        <v>13.4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="15" thickBot="1">
-      <c r="A44" s="3">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="15" thickBot="1">
-      <c r="A45" s="3">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="15" thickBot="1">
-      <c r="A46" s="4">
-        <v>14.9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="15" thickBot="1">
-      <c r="A47" s="4">
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="15" thickBot="1">
-      <c r="A48" s="4">
-        <v>14.9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="15" thickBot="1">
-      <c r="A49" s="4">
-        <v>15.1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="15" thickBot="1">
-      <c r="A50" s="4">
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="15" thickBot="1">
-      <c r="A51" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="15" thickBot="1">
-      <c r="A52" s="4">
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="15" thickBot="1">
-      <c r="A53" s="3">
-        <v>12.7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="15" thickBot="1">
-      <c r="A54" s="3">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="15" thickBot="1">
-      <c r="A55" s="2">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="15" thickBot="1">
-      <c r="A56" s="3">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="15" thickBot="1">
-      <c r="A57" s="3">
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="15" thickBot="1">
-      <c r="A58" s="4">
-        <v>14.3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="15" thickBot="1">
-      <c r="A59" s="3">
+      <c r="E100" s="16">
+        <v>23</v>
+      </c>
+      <c r="F100" s="14">
+        <v>3</v>
+      </c>
+      <c r="G100" s="17">
         <v>13</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" ht="15" thickBot="1">
-      <c r="A60" s="4">
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="15" thickBot="1">
-      <c r="A61" s="3">
-        <v>12.6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="15" thickBot="1">
-      <c r="A62" s="4">
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" ht="15" thickBot="1">
-      <c r="A63" s="3">
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" ht="15" thickBot="1">
-      <c r="A64" s="4">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" ht="15" thickBot="1">
-      <c r="A65" s="3">
-        <v>12.9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" ht="15" thickBot="1">
-      <c r="A66" s="4">
-        <v>14.1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="15" thickBot="1">
-      <c r="A67" s="4">
-        <v>14.9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="15" thickBot="1">
-      <c r="A68" s="4">
-        <v>14.2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" ht="15" thickBot="1">
-      <c r="A69" s="4">
-        <v>14.9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" ht="15" thickBot="1">
-      <c r="A70" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" ht="15" thickBot="1">
-      <c r="A71" s="4">
-        <v>15.1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="15" thickBot="1">
-      <c r="A72" s="3">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="15" thickBot="1">
-      <c r="A73" s="3">
-        <v>11.7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" ht="15" thickBot="1">
-      <c r="A74" s="3">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="15" thickBot="1">
-      <c r="A75" s="4">
-        <v>14.6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" ht="15" thickBot="1">
-      <c r="A76" s="7">
+      <c r="H100">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="15" thickBot="1">
+      <c r="A101">
+        <v>2020</v>
+      </c>
+      <c r="B101" s="10">
+        <v>67</v>
+      </c>
+      <c r="C101" s="13">
+        <v>61</v>
+      </c>
+      <c r="D101" s="15">
+        <v>104</v>
+      </c>
+      <c r="E101" s="18">
+        <v>51</v>
+      </c>
+      <c r="F101" s="25">
+        <v>143</v>
+      </c>
+      <c r="G101" s="20">
+        <v>131</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="1"/>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="15" thickBot="1">
+      <c r="A102">
+        <v>2021</v>
+      </c>
+      <c r="B102" s="23">
+        <v>116</v>
+      </c>
+      <c r="C102" s="24">
+        <v>77</v>
+      </c>
+      <c r="D102" s="16">
         <v>17</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" ht="15" thickBot="1">
-      <c r="A77" s="4">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" ht="15" thickBot="1">
-      <c r="A78" s="4">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" ht="15" thickBot="1">
-      <c r="A79" s="4">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" ht="15" thickBot="1">
-      <c r="A80" s="4">
-        <v>14.6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="15" thickBot="1">
-      <c r="A81" s="4">
-        <v>14.1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" ht="15" thickBot="1">
-      <c r="A82" s="7">
-        <v>16.8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" ht="15" thickBot="1">
-      <c r="A83" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" ht="15" thickBot="1">
-      <c r="A84" s="3">
-        <v>12.9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" ht="15" thickBot="1">
-      <c r="A85" s="4">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" ht="15" thickBot="1">
-      <c r="A86" s="4">
-        <v>16.399999999999999</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" ht="15" thickBot="1">
-      <c r="A87" s="7">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" ht="15" thickBot="1">
-      <c r="A88" s="3">
-        <v>13.4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" ht="15" thickBot="1">
-      <c r="A89" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" ht="15" thickBot="1">
-      <c r="A90" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" ht="15" thickBot="1">
-      <c r="A91" s="4">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" ht="15" thickBot="1">
-      <c r="A92" s="4">
-        <v>14.8</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" ht="15" thickBot="1">
-      <c r="A93" s="4">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" ht="15" thickBot="1">
-      <c r="A94" s="4">
-        <v>15.9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" ht="15" thickBot="1">
-      <c r="A95" s="7">
-        <v>16.7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" ht="15" thickBot="1">
-      <c r="A96" s="3">
-        <v>13.3</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" ht="15" thickBot="1">
-      <c r="A97" s="3">
-        <v>13.3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" ht="15" thickBot="1">
-      <c r="A98" s="4">
-        <v>15.6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" ht="15" thickBot="1">
-      <c r="A99" s="4">
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" ht="15" thickBot="1">
-      <c r="A100" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" ht="15" thickBot="1">
-      <c r="A101" s="4">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" ht="15" thickBot="1">
-      <c r="A102" s="4">
-        <v>14.1</v>
+      <c r="E102" s="27">
+        <v>166</v>
+      </c>
+      <c r="F102" s="16">
+        <v>17</v>
+      </c>
+      <c r="G102" s="34">
+        <v>231</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="1"/>
+        <v>624</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reformatting data, price predictions
</commit_message>
<xml_diff>
--- a/data/bordeauxWeather.xlsx
+++ b/data/bordeauxWeather.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polin\Dropbox\EE 608 spring 2023\project\Wine-Quality-Modeling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA673005-1110-44C0-9092-1F78BA91C66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F89F9DC-9EE9-4A4F-9A13-1EDE908CA034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12660" yWindow="0" windowWidth="18048" windowHeight="16680" activeTab="1" xr2:uid="{D0F1188E-B2DB-4E86-B194-F78466D191BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{D0F1188E-B2DB-4E86-B194-F78466D191BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="2" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>year</t>
   </si>
@@ -122,12 +125,27 @@
   <si>
     <t>decP</t>
   </si>
+  <si>
+    <t>ashNoYr</t>
+  </si>
+  <si>
+    <t>ashYr</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,15 +172,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF282828"/>
+      <name val="Calibri "/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri "/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri "/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,8 +404,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -408,11 +444,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -525,17 +577,28 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -853,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B54E63-F438-48F7-83CF-1118160EA2FA}">
-  <dimension ref="A1:Y102"/>
+  <dimension ref="A1:AD102"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A18" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG11" sqref="AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -867,7 +930,7 @@
     <col min="25" max="25" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" thickBot="1">
+    <row r="1" spans="1:30" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -940,8 +1003,21 @@
       <c r="Y1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" ht="15" thickBot="1">
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="15" thickBot="1">
       <c r="A2">
         <v>1921</v>
       </c>
@@ -1017,8 +1093,22 @@
         <f>SUM(K2:M2)+74+32+12</f>
         <v>243</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="15" thickBot="1">
+      <c r="AA2">
+        <f>0.608*I2-0.0038*X2+0.00115*Y2+0.00765*G2</f>
+        <v>11.215106666666669</v>
+      </c>
+      <c r="AB2">
+        <f>0.24*(2021-A2)+0.608*I2-0.0038*X2+0.00115*Y2+0.00765*G2</f>
+        <v>35.215106666666664</v>
+      </c>
+      <c r="AC2" s="41">
+        <v>3503</v>
+      </c>
+      <c r="AD2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="15" thickBot="1">
       <c r="A3">
         <v>1922</v>
       </c>
@@ -1094,8 +1184,22 @@
         <f>SUM(K3:M3)+SUM(T2:V2)</f>
         <v>289</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="15" thickBot="1">
+      <c r="AA3">
+        <f t="shared" ref="AA3:AA66" si="2">0.608*I3-0.0038*X3+0.00115*Y3+0.00765*G3</f>
+        <v>9.9253283333333293</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB66" si="3">0.24*(2021-A3)+0.608*I3-0.0038*X3+0.00115*Y3+0.00765*G3</f>
+        <v>33.685328333333324</v>
+      </c>
+      <c r="AC3" s="41">
+        <v>3002</v>
+      </c>
+      <c r="AD3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="15" thickBot="1">
       <c r="A4">
         <v>1923</v>
       </c>
@@ -1168,11 +1272,25 @@
         <v>67</v>
       </c>
       <c r="Y4">
-        <f t="shared" ref="Y4:Y67" si="2">SUM(K4:M4)+SUM(T3:V3)</f>
+        <f t="shared" ref="Y4:Y67" si="4">SUM(K4:M4)+SUM(T3:V3)</f>
         <v>489</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" ht="15" thickBot="1">
+      <c r="AA4">
+        <f t="shared" si="2"/>
+        <v>10.0223975</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="3"/>
+        <v>33.5423975</v>
+      </c>
+      <c r="AC4" s="41">
+        <v>2471</v>
+      </c>
+      <c r="AD4">
+        <v>0.80500000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="15" thickBot="1">
       <c r="A5">
         <v>1924</v>
       </c>
@@ -1245,11 +1363,25 @@
         <v>139</v>
       </c>
       <c r="Y5">
+        <f t="shared" si="4"/>
+        <v>590</v>
+      </c>
+      <c r="AA5">
         <f t="shared" si="2"/>
-        <v>590</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="15" thickBot="1">
+        <v>9.3292166666666638</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="3"/>
+        <v>32.609216666666661</v>
+      </c>
+      <c r="AC5" s="41">
+        <v>1940</v>
+      </c>
+      <c r="AD5">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="15" thickBot="1">
       <c r="A6">
         <v>1925</v>
       </c>
@@ -1322,11 +1454,25 @@
         <v>104</v>
       </c>
       <c r="Y6">
+        <f t="shared" si="4"/>
+        <v>504</v>
+      </c>
+      <c r="AA6">
         <f t="shared" si="2"/>
-        <v>504</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="15" thickBot="1">
+        <v>10.317003333333332</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="3"/>
+        <v>33.357003333333324</v>
+      </c>
+      <c r="AC6" s="41">
+        <v>2346</v>
+      </c>
+      <c r="AD6">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="15" thickBot="1">
       <c r="A7">
         <v>1926</v>
       </c>
@@ -1399,11 +1545,25 @@
         <v>68</v>
       </c>
       <c r="Y7">
+        <f t="shared" si="4"/>
+        <v>502</v>
+      </c>
+      <c r="AA7">
         <f t="shared" si="2"/>
-        <v>502</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="15" thickBot="1">
+        <v>10.758186666666665</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="3"/>
+        <v>33.558186666666664</v>
+      </c>
+      <c r="AC7" s="41">
+        <v>2752</v>
+      </c>
+      <c r="AD7">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="15" thickBot="1">
       <c r="A8">
         <v>1927</v>
       </c>
@@ -1476,11 +1636,25 @@
         <v>171</v>
       </c>
       <c r="Y8">
+        <f t="shared" si="4"/>
+        <v>656</v>
+      </c>
+      <c r="AA8">
         <f t="shared" si="2"/>
-        <v>656</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="15" thickBot="1">
+        <v>10.199729999999999</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="3"/>
+        <v>32.759729999999998</v>
+      </c>
+      <c r="AC8" s="41">
+        <v>2713.5</v>
+      </c>
+      <c r="AD8">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="15" thickBot="1">
       <c r="A9">
         <v>1928</v>
       </c>
@@ -1553,11 +1727,25 @@
         <v>77</v>
       </c>
       <c r="Y9">
+        <f t="shared" si="4"/>
+        <v>492</v>
+      </c>
+      <c r="AA9">
         <f t="shared" si="2"/>
-        <v>492</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="15" thickBot="1">
+        <v>10.825671666666667</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="3"/>
+        <v>33.145671666666665</v>
+      </c>
+      <c r="AC9" s="41">
+        <v>2675</v>
+      </c>
+      <c r="AD9">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="15" thickBot="1">
       <c r="A10">
         <v>1929</v>
       </c>
@@ -1630,11 +1818,25 @@
         <v>37</v>
       </c>
       <c r="Y10">
+        <f t="shared" si="4"/>
+        <v>460.4</v>
+      </c>
+      <c r="AA10">
         <f t="shared" si="2"/>
-        <v>460.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="15" thickBot="1">
+        <v>10.798323333333334</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="3"/>
+        <v>32.878323333333334</v>
+      </c>
+      <c r="AC10" s="41">
+        <v>2831</v>
+      </c>
+      <c r="AD10">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="15" thickBot="1">
       <c r="A11">
         <v>1930</v>
       </c>
@@ -1707,11 +1909,25 @@
         <v>119</v>
       </c>
       <c r="Y11">
+        <f t="shared" si="4"/>
+        <v>706</v>
+      </c>
+      <c r="AA11">
         <f t="shared" si="2"/>
-        <v>706</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="15" thickBot="1">
+        <v>10.384473333333332</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="3"/>
+        <v>32.224473333333329</v>
+      </c>
+      <c r="AC11" s="41">
+        <v>3426</v>
+      </c>
+      <c r="AD11">
+        <v>0.79500000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="15" thickBot="1">
       <c r="A12">
         <v>1931</v>
       </c>
@@ -1784,11 +2000,25 @@
         <v>298</v>
       </c>
       <c r="Y12">
+        <f t="shared" si="4"/>
+        <v>867</v>
+      </c>
+      <c r="AA12">
         <f t="shared" si="2"/>
-        <v>867</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="15" thickBot="1">
+        <v>9.5135249999999996</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="3"/>
+        <v>31.113524999999999</v>
+      </c>
+      <c r="AC12" s="41">
+        <v>4021</v>
+      </c>
+      <c r="AD12">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="15" thickBot="1">
       <c r="A13">
         <v>1932</v>
       </c>
@@ -1861,11 +2091,25 @@
         <v>246</v>
       </c>
       <c r="Y13">
+        <f t="shared" si="4"/>
+        <v>346</v>
+      </c>
+      <c r="AA13">
         <f t="shared" si="2"/>
-        <v>346</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="15" thickBot="1">
+        <v>9.4830950000000005</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="3"/>
+        <v>30.843094999999998</v>
+      </c>
+      <c r="AC13" s="41">
+        <v>2950.5</v>
+      </c>
+      <c r="AD13">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="15" thickBot="1">
       <c r="A14">
         <v>1933</v>
       </c>
@@ -1938,11 +2182,25 @@
         <v>184</v>
       </c>
       <c r="Y14">
+        <f t="shared" si="4"/>
+        <v>445</v>
+      </c>
+      <c r="AA14">
         <f t="shared" si="2"/>
-        <v>445</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="15" thickBot="1">
+        <v>10.635373333333332</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="3"/>
+        <v>31.755373333333328</v>
+      </c>
+      <c r="AC14" s="41">
+        <v>1880</v>
+      </c>
+      <c r="AD14">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" ht="15" thickBot="1">
       <c r="A15">
         <v>1934</v>
       </c>
@@ -2015,11 +2273,25 @@
         <v>134</v>
       </c>
       <c r="Y15">
+        <f t="shared" si="4"/>
+        <v>539</v>
+      </c>
+      <c r="AA15">
         <f t="shared" si="2"/>
-        <v>539</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="15" thickBot="1">
+        <v>10.989495</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="3"/>
+        <v>31.869494999999997</v>
+      </c>
+      <c r="AC15" s="41">
+        <v>1537</v>
+      </c>
+      <c r="AD15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="15" thickBot="1">
       <c r="A16">
         <v>1935</v>
       </c>
@@ -2092,11 +2364,25 @@
         <v>137</v>
       </c>
       <c r="Y16">
+        <f t="shared" si="4"/>
+        <v>576</v>
+      </c>
+      <c r="AA16">
         <f t="shared" si="2"/>
-        <v>576</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" ht="15" thickBot="1">
+        <v>10.506328333333334</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" si="3"/>
+        <v>31.146328333333333</v>
+      </c>
+      <c r="AC16" s="41">
+        <v>1687.666666666667</v>
+      </c>
+      <c r="AD16">
+        <v>0.89333333333333331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" ht="15" thickBot="1">
       <c r="A17">
         <v>1936</v>
       </c>
@@ -2169,11 +2455,25 @@
         <v>29</v>
       </c>
       <c r="Y17">
+        <f t="shared" si="4"/>
+        <v>780</v>
+      </c>
+      <c r="AA17">
         <f t="shared" si="2"/>
-        <v>780</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" ht="15" thickBot="1">
+        <v>10.544281666666667</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="3"/>
+        <v>30.944281666666662</v>
+      </c>
+      <c r="AC17" s="41">
+        <v>1838.3333333333339</v>
+      </c>
+      <c r="AD17">
+        <v>0.88666666666666671</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="15" thickBot="1">
       <c r="A18">
         <v>1937</v>
       </c>
@@ -2246,11 +2546,25 @@
         <v>154</v>
       </c>
       <c r="Y18">
+        <f t="shared" si="4"/>
+        <v>459</v>
+      </c>
+      <c r="AA18">
         <f t="shared" si="2"/>
-        <v>459</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" ht="15" thickBot="1">
+        <v>10.358033333333335</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="3"/>
+        <v>30.518033333333335</v>
+      </c>
+      <c r="AC18" s="41">
+        <v>1989.0000000000009</v>
+      </c>
+      <c r="AD18">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" ht="15" thickBot="1">
       <c r="A19">
         <v>1938</v>
       </c>
@@ -2323,11 +2637,25 @@
         <v>142</v>
       </c>
       <c r="Y19">
+        <f t="shared" si="4"/>
+        <v>548</v>
+      </c>
+      <c r="AA19">
         <f t="shared" si="2"/>
-        <v>548</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" ht="15" thickBot="1">
+        <v>9.8754216666666661</v>
+      </c>
+      <c r="AB19">
+        <f t="shared" si="3"/>
+        <v>29.795421666666662</v>
+      </c>
+      <c r="AC19" s="41">
+        <v>1990.0000000000009</v>
+      </c>
+      <c r="AD19">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" ht="15" thickBot="1">
       <c r="A20">
         <v>1939</v>
       </c>
@@ -2400,11 +2728,25 @@
         <v>91</v>
       </c>
       <c r="Y20">
+        <f t="shared" si="4"/>
+        <v>537</v>
+      </c>
+      <c r="AA20">
         <f t="shared" si="2"/>
-        <v>537</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" ht="15" thickBot="1">
+        <v>10.076838333333335</v>
+      </c>
+      <c r="AB20">
+        <f t="shared" si="3"/>
+        <v>29.756838333333338</v>
+      </c>
+      <c r="AC20" s="41">
+        <v>681</v>
+      </c>
+      <c r="AD20">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" ht="15" thickBot="1">
       <c r="A21">
         <v>1940</v>
       </c>
@@ -2477,11 +2819,25 @@
         <v>88</v>
       </c>
       <c r="Y21">
+        <f t="shared" si="4"/>
+        <v>489</v>
+      </c>
+      <c r="AA21">
         <f t="shared" si="2"/>
-        <v>489</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" ht="15" thickBot="1">
+        <v>10.236469999999999</v>
+      </c>
+      <c r="AB21">
+        <f t="shared" si="3"/>
+        <v>29.676469999999998</v>
+      </c>
+      <c r="AC21" s="41">
+        <v>2012</v>
+      </c>
+      <c r="AD21">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" ht="15" thickBot="1">
       <c r="A22">
         <v>1941</v>
       </c>
@@ -2554,11 +2910,25 @@
         <v>212</v>
       </c>
       <c r="Y22">
+        <f t="shared" si="4"/>
+        <v>637</v>
+      </c>
+      <c r="AA22">
         <f t="shared" si="2"/>
-        <v>637</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" ht="15" thickBot="1">
+        <v>10.286083333333332</v>
+      </c>
+      <c r="AB22">
+        <f t="shared" si="3"/>
+        <v>29.486083333333337</v>
+      </c>
+      <c r="AC22" s="41">
+        <v>1727.5</v>
+      </c>
+      <c r="AD22">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" ht="15" thickBot="1">
       <c r="A23">
         <v>1942</v>
       </c>
@@ -2631,11 +3001,25 @@
         <v>200</v>
       </c>
       <c r="Y23">
+        <f t="shared" si="4"/>
+        <v>290</v>
+      </c>
+      <c r="AA23">
         <f t="shared" si="2"/>
-        <v>290</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" ht="15" thickBot="1">
+        <v>10.283246666666667</v>
+      </c>
+      <c r="AB23">
+        <f t="shared" si="3"/>
+        <v>29.243246666666668</v>
+      </c>
+      <c r="AC23" s="41">
+        <v>1443</v>
+      </c>
+      <c r="AD23">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" ht="15" thickBot="1">
       <c r="A24">
         <v>1943</v>
       </c>
@@ -2708,11 +3092,25 @@
         <v>129</v>
       </c>
       <c r="Y24">
+        <f t="shared" si="4"/>
+        <v>318</v>
+      </c>
+      <c r="AA24">
         <f t="shared" si="2"/>
-        <v>318</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" ht="15" thickBot="1">
+        <v>10.93586</v>
+      </c>
+      <c r="AB24">
+        <f t="shared" si="3"/>
+        <v>29.655860000000001</v>
+      </c>
+      <c r="AC24" s="41">
+        <v>1985</v>
+      </c>
+      <c r="AD24">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" ht="15" thickBot="1">
       <c r="A25">
         <v>1944</v>
       </c>
@@ -2785,11 +3183,25 @@
         <v>153</v>
       </c>
       <c r="Y25">
+        <f t="shared" si="4"/>
+        <v>311</v>
+      </c>
+      <c r="AA25">
         <f t="shared" si="2"/>
-        <v>311</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" ht="15" thickBot="1">
+        <v>11.187223333333332</v>
+      </c>
+      <c r="AB25">
+        <f t="shared" si="3"/>
+        <v>29.667223333333336</v>
+      </c>
+      <c r="AC25" s="41">
+        <v>2129</v>
+      </c>
+      <c r="AD25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" ht="15" thickBot="1">
       <c r="A26">
         <v>1945</v>
       </c>
@@ -2862,11 +3274,25 @@
         <v>90</v>
       </c>
       <c r="Y26">
+        <f t="shared" si="4"/>
+        <v>536</v>
+      </c>
+      <c r="AA26">
         <f t="shared" si="2"/>
-        <v>536</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" ht="15" thickBot="1">
+        <v>12.090478333333333</v>
+      </c>
+      <c r="AB26">
+        <f t="shared" si="3"/>
+        <v>30.330478333333332</v>
+      </c>
+      <c r="AC26" s="41">
+        <v>2938</v>
+      </c>
+      <c r="AD26">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" ht="15" thickBot="1">
       <c r="A27">
         <v>1946</v>
       </c>
@@ -2939,11 +3365,25 @@
         <v>98</v>
       </c>
       <c r="Y27">
+        <f t="shared" si="4"/>
+        <v>335</v>
+      </c>
+      <c r="AA27">
         <f t="shared" si="2"/>
-        <v>335</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" ht="15" thickBot="1">
+        <v>10.137426666666665</v>
+      </c>
+      <c r="AB27">
+        <f t="shared" si="3"/>
+        <v>28.137426666666666</v>
+      </c>
+      <c r="AC27" s="41">
+        <v>5285</v>
+      </c>
+      <c r="AD27">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" ht="15" thickBot="1">
       <c r="A28">
         <v>1947</v>
       </c>
@@ -3016,11 +3456,25 @@
         <v>138</v>
       </c>
       <c r="Y28">
+        <f t="shared" si="4"/>
+        <v>592</v>
+      </c>
+      <c r="AA28">
         <f t="shared" si="2"/>
-        <v>592</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" ht="15" thickBot="1">
+        <v>11.582445</v>
+      </c>
+      <c r="AB28">
+        <f t="shared" si="3"/>
+        <v>29.342444999999998</v>
+      </c>
+      <c r="AC28" s="41">
+        <v>1616</v>
+      </c>
+      <c r="AD28">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" ht="15" thickBot="1">
       <c r="A29">
         <v>1948</v>
       </c>
@@ -3093,11 +3547,25 @@
         <v>106</v>
       </c>
       <c r="Y29">
+        <f t="shared" si="4"/>
+        <v>485</v>
+      </c>
+      <c r="AA29">
         <f t="shared" si="2"/>
-        <v>485</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" ht="15" thickBot="1">
+        <v>10.401126666666665</v>
+      </c>
+      <c r="AB29">
+        <f t="shared" si="3"/>
+        <v>27.921126666666662</v>
+      </c>
+      <c r="AC29" s="41">
+        <v>1870</v>
+      </c>
+      <c r="AD29">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" ht="15" thickBot="1">
       <c r="A30">
         <v>1949</v>
       </c>
@@ -3170,11 +3638,25 @@
         <v>90</v>
       </c>
       <c r="Y30">
+        <f t="shared" si="4"/>
+        <v>256</v>
+      </c>
+      <c r="AA30">
         <f t="shared" si="2"/>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" ht="15" thickBot="1">
+        <v>11.269849999999998</v>
+      </c>
+      <c r="AB30">
+        <f t="shared" si="3"/>
+        <v>28.549849999999999</v>
+      </c>
+      <c r="AC30" s="41">
+        <v>1920</v>
+      </c>
+      <c r="AD30">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" ht="15" thickBot="1">
       <c r="A31">
         <v>1950</v>
       </c>
@@ -3247,11 +3729,25 @@
         <v>136</v>
       </c>
       <c r="Y31">
+        <f t="shared" si="4"/>
+        <v>567</v>
+      </c>
+      <c r="AA31">
         <f t="shared" si="2"/>
-        <v>567</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" ht="15" thickBot="1">
+        <v>10.807979999999999</v>
+      </c>
+      <c r="AB31">
+        <f t="shared" si="3"/>
+        <v>27.84798</v>
+      </c>
+      <c r="AC31" s="41">
+        <v>1566</v>
+      </c>
+      <c r="AD31">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" ht="15" thickBot="1">
       <c r="A32">
         <v>1951</v>
       </c>
@@ -3324,11 +3820,25 @@
         <v>177</v>
       </c>
       <c r="Y32">
+        <f t="shared" si="4"/>
+        <v>747</v>
+      </c>
+      <c r="AA32">
         <f t="shared" si="2"/>
-        <v>747</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" ht="15" thickBot="1">
+        <v>10.090388333333337</v>
+      </c>
+      <c r="AB32">
+        <f t="shared" si="3"/>
+        <v>26.890388333333334</v>
+      </c>
+      <c r="AC32" s="41">
+        <v>2375</v>
+      </c>
+      <c r="AD32">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" ht="15" thickBot="1">
       <c r="A33">
         <v>1952</v>
       </c>
@@ -3401,11 +3911,25 @@
         <v>166</v>
       </c>
       <c r="Y33">
+        <f t="shared" si="4"/>
+        <v>566</v>
+      </c>
+      <c r="AA33">
         <f t="shared" si="2"/>
-        <v>566</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" ht="15" thickBot="1">
+        <v>10.536428333333332</v>
+      </c>
+      <c r="AB33">
+        <f t="shared" si="3"/>
+        <v>27.096428333333328</v>
+      </c>
+      <c r="AC33" s="41">
+        <v>1253</v>
+      </c>
+      <c r="AD33">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" ht="15" thickBot="1">
       <c r="A34">
         <v>1953</v>
       </c>
@@ -3478,11 +4002,25 @@
         <v>76</v>
       </c>
       <c r="Y34">
+        <f t="shared" si="4"/>
+        <v>653</v>
+      </c>
+      <c r="AA34">
         <f t="shared" si="2"/>
-        <v>653</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" ht="15" thickBot="1">
+        <v>10.768361666666665</v>
+      </c>
+      <c r="AB34">
+        <f t="shared" si="3"/>
+        <v>27.088361666666668</v>
+      </c>
+      <c r="AC34" s="41">
+        <v>2692</v>
+      </c>
+      <c r="AD34">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" ht="15" thickBot="1">
       <c r="A35">
         <v>1954</v>
       </c>
@@ -3555,11 +4093,25 @@
         <v>171</v>
       </c>
       <c r="Y35">
+        <f t="shared" si="4"/>
+        <v>414</v>
+      </c>
+      <c r="AA35">
         <f t="shared" si="2"/>
-        <v>414</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" ht="15" thickBot="1">
+        <v>9.3078866666666666</v>
+      </c>
+      <c r="AB35">
+        <f t="shared" si="3"/>
+        <v>25.387886666666667</v>
+      </c>
+      <c r="AC35" s="41">
+        <v>1568</v>
+      </c>
+      <c r="AD35">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" ht="15" thickBot="1">
       <c r="A36">
         <v>1955</v>
       </c>
@@ -3632,11 +4184,25 @@
         <v>130</v>
       </c>
       <c r="Y36">
+        <f t="shared" si="4"/>
+        <v>505</v>
+      </c>
+      <c r="AA36">
         <f t="shared" si="2"/>
-        <v>505</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" ht="15" thickBot="1">
+        <v>10.642469999999999</v>
+      </c>
+      <c r="AB36">
+        <f t="shared" si="3"/>
+        <v>26.482469999999999</v>
+      </c>
+      <c r="AC36" s="41">
+        <v>2039</v>
+      </c>
+      <c r="AD36">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" ht="15" thickBot="1">
       <c r="A37">
         <v>1956</v>
       </c>
@@ -3709,11 +4275,25 @@
         <v>140</v>
       </c>
       <c r="Y37">
+        <f t="shared" si="4"/>
+        <v>397</v>
+      </c>
+      <c r="AA37">
         <f t="shared" si="2"/>
-        <v>397</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" ht="15" thickBot="1">
+        <v>9.5822283333333331</v>
+      </c>
+      <c r="AB37">
+        <f t="shared" si="3"/>
+        <v>25.182228333333331</v>
+      </c>
+      <c r="AC37" s="41">
+        <v>1589</v>
+      </c>
+      <c r="AD37">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" ht="15" thickBot="1">
       <c r="A38">
         <v>1957</v>
       </c>
@@ -3786,11 +4366,25 @@
         <v>110</v>
       </c>
       <c r="Y38">
+        <f t="shared" si="4"/>
+        <v>391</v>
+      </c>
+      <c r="AA38">
         <f t="shared" si="2"/>
-        <v>391</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" ht="15" thickBot="1">
+        <v>9.9646466666666687</v>
+      </c>
+      <c r="AB38">
+        <f t="shared" si="3"/>
+        <v>25.324646666666666</v>
+      </c>
+      <c r="AC38" s="41">
+        <v>1003</v>
+      </c>
+      <c r="AD38">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" ht="15" thickBot="1">
       <c r="A39">
         <v>1958</v>
       </c>
@@ -3863,11 +4457,25 @@
         <v>187</v>
       </c>
       <c r="Y39">
+        <f t="shared" si="4"/>
+        <v>540</v>
+      </c>
+      <c r="AA39">
         <f t="shared" si="2"/>
-        <v>540</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" ht="15" thickBot="1">
+        <v>10.037848333333335</v>
+      </c>
+      <c r="AB39">
+        <f t="shared" si="3"/>
+        <v>25.157848333333334</v>
+      </c>
+      <c r="AC39" s="41">
+        <v>1193</v>
+      </c>
+      <c r="AD39">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" ht="15" thickBot="1">
       <c r="A40">
         <v>1959</v>
       </c>
@@ -3940,11 +4548,25 @@
         <v>183</v>
       </c>
       <c r="Y40">
+        <f t="shared" si="4"/>
+        <v>378</v>
+      </c>
+      <c r="AA40">
         <f t="shared" si="2"/>
-        <v>378</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" ht="15" thickBot="1">
+        <v>10.512221666666667</v>
+      </c>
+      <c r="AB40">
+        <f t="shared" si="3"/>
+        <v>25.392221666666668</v>
+      </c>
+      <c r="AC40" s="41">
+        <v>6425</v>
+      </c>
+      <c r="AD40">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" ht="15" thickBot="1">
       <c r="A41">
         <v>1960</v>
       </c>
@@ -4017,11 +4639,25 @@
         <v>290</v>
       </c>
       <c r="Y41">
+        <f t="shared" si="4"/>
+        <v>748</v>
+      </c>
+      <c r="AA41">
         <f t="shared" si="2"/>
-        <v>748</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" ht="15" thickBot="1">
+        <v>9.8604033333333341</v>
+      </c>
+      <c r="AB41">
+        <f t="shared" si="3"/>
+        <v>24.500403333333331</v>
+      </c>
+      <c r="AC41" s="41">
+        <v>960</v>
+      </c>
+      <c r="AD41">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" ht="15" thickBot="1">
       <c r="A42">
         <v>1961</v>
       </c>
@@ -4094,11 +4730,25 @@
         <v>38</v>
       </c>
       <c r="Y42">
+        <f t="shared" si="4"/>
+        <v>748</v>
+      </c>
+      <c r="AA42">
         <f t="shared" si="2"/>
-        <v>748</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" ht="15" thickBot="1">
+        <v>11.369228333333334</v>
+      </c>
+      <c r="AB42">
+        <f t="shared" si="3"/>
+        <v>25.769228333333327</v>
+      </c>
+      <c r="AC42" s="41">
+        <v>2706</v>
+      </c>
+      <c r="AD42">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" ht="15" thickBot="1">
       <c r="A43">
         <v>1962</v>
       </c>
@@ -4171,11 +4821,25 @@
         <v>52</v>
       </c>
       <c r="Y43">
+        <f t="shared" si="4"/>
+        <v>640</v>
+      </c>
+      <c r="AA43">
         <f t="shared" si="2"/>
-        <v>640</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" ht="15" thickBot="1">
+        <v>10.54998</v>
+      </c>
+      <c r="AB43">
+        <f t="shared" si="3"/>
+        <v>24.709979999999998</v>
+      </c>
+      <c r="AC43" s="41">
+        <v>1469</v>
+      </c>
+      <c r="AD43">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" ht="15" thickBot="1">
       <c r="A44">
         <v>1963</v>
       </c>
@@ -4248,11 +4912,25 @@
         <v>155</v>
       </c>
       <c r="Y44">
+        <f t="shared" si="4"/>
+        <v>566</v>
+      </c>
+      <c r="AA44">
         <f t="shared" si="2"/>
-        <v>566</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25" ht="15" thickBot="1">
+        <v>9.7111633333333316</v>
+      </c>
+      <c r="AB44">
+        <f t="shared" si="3"/>
+        <v>23.631163333333333</v>
+      </c>
+      <c r="AC44" s="41">
+        <v>2323</v>
+      </c>
+      <c r="AD44">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" ht="15" thickBot="1">
       <c r="A45">
         <v>1964</v>
       </c>
@@ -4325,11 +5003,25 @@
         <v>96</v>
       </c>
       <c r="Y45">
+        <f t="shared" si="4"/>
+        <v>327</v>
+      </c>
+      <c r="AA45">
         <f t="shared" si="2"/>
-        <v>327</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" ht="15" thickBot="1">
+        <v>10.622038333333334</v>
+      </c>
+      <c r="AB45">
+        <f t="shared" si="3"/>
+        <v>24.302038333333336</v>
+      </c>
+      <c r="AC45" s="41">
+        <v>838</v>
+      </c>
+      <c r="AD45">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" ht="15" thickBot="1">
       <c r="A46">
         <v>1965</v>
       </c>
@@ -4402,11 +5094,25 @@
         <v>267</v>
       </c>
       <c r="Y46">
+        <f t="shared" si="4"/>
+        <v>549</v>
+      </c>
+      <c r="AA46">
         <f t="shared" si="2"/>
-        <v>549</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" ht="15" thickBot="1">
+        <v>9.0417383333333348</v>
+      </c>
+      <c r="AB46">
+        <f t="shared" si="3"/>
+        <v>22.481738333333332</v>
+      </c>
+      <c r="AC46" s="41">
+        <v>927</v>
+      </c>
+      <c r="AD46">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" ht="15" thickBot="1">
       <c r="A47">
         <v>1966</v>
       </c>
@@ -4479,11 +5185,25 @@
         <v>86</v>
       </c>
       <c r="Y47">
+        <f t="shared" si="4"/>
+        <v>735</v>
+      </c>
+      <c r="AA47">
         <f t="shared" si="2"/>
-        <v>735</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" ht="15" thickBot="1">
+        <v>10.660045</v>
+      </c>
+      <c r="AB47">
+        <f t="shared" si="3"/>
+        <v>23.860045</v>
+      </c>
+      <c r="AC47" s="41">
+        <v>1033</v>
+      </c>
+      <c r="AD47">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" ht="15" thickBot="1">
       <c r="A48">
         <v>1967</v>
       </c>
@@ -4556,11 +5276,25 @@
         <v>118</v>
       </c>
       <c r="Y48">
+        <f t="shared" si="4"/>
+        <v>647</v>
+      </c>
+      <c r="AA48">
         <f t="shared" si="2"/>
-        <v>647</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" ht="15" thickBot="1">
+        <v>10.251208333333334</v>
+      </c>
+      <c r="AB48">
+        <f t="shared" si="3"/>
+        <v>23.211208333333335</v>
+      </c>
+      <c r="AC48" s="41">
+        <v>684</v>
+      </c>
+      <c r="AD48">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" ht="15" thickBot="1">
       <c r="A49">
         <v>1968</v>
       </c>
@@ -4633,11 +5367,25 @@
         <v>292</v>
       </c>
       <c r="Y49">
+        <f t="shared" si="4"/>
+        <v>509</v>
+      </c>
+      <c r="AA49">
         <f t="shared" si="2"/>
-        <v>509</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" ht="15" thickBot="1">
+        <v>9.4305433333333344</v>
+      </c>
+      <c r="AB49">
+        <f t="shared" si="3"/>
+        <v>22.150543333333335</v>
+      </c>
+      <c r="AC49" s="41">
+        <v>1446</v>
+      </c>
+      <c r="AD49">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" ht="15" thickBot="1">
       <c r="A50">
         <v>1969</v>
       </c>
@@ -4710,11 +5458,25 @@
         <v>244</v>
       </c>
       <c r="Y50">
+        <f t="shared" si="4"/>
+        <v>481</v>
+      </c>
+      <c r="AA50">
         <f t="shared" si="2"/>
-        <v>481</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" ht="15" thickBot="1">
+        <v>9.7841750000000012</v>
+      </c>
+      <c r="AB50">
+        <f t="shared" si="3"/>
+        <v>22.264175000000002</v>
+      </c>
+      <c r="AC50" s="41">
+        <v>855</v>
+      </c>
+      <c r="AD50">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:30" ht="15" thickBot="1">
       <c r="A51">
         <v>1970</v>
       </c>
@@ -4787,11 +5549,25 @@
         <v>89</v>
       </c>
       <c r="Y51">
+        <f t="shared" si="4"/>
+        <v>563</v>
+      </c>
+      <c r="AA51">
         <f t="shared" si="2"/>
-        <v>563</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" ht="15" thickBot="1">
+        <v>10.549118333333329</v>
+      </c>
+      <c r="AB51">
+        <f t="shared" si="3"/>
+        <v>22.789118333333331</v>
+      </c>
+      <c r="AC51" s="41">
+        <v>742</v>
+      </c>
+      <c r="AD51">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:30" ht="15" thickBot="1">
       <c r="A52">
         <v>1971</v>
       </c>
@@ -4864,11 +5640,25 @@
         <v>112</v>
       </c>
       <c r="Y52">
+        <f t="shared" si="4"/>
+        <v>488</v>
+      </c>
+      <c r="AA52">
         <f t="shared" si="2"/>
-        <v>488</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" ht="15" thickBot="1">
+        <v>10.459018333333333</v>
+      </c>
+      <c r="AB52">
+        <f t="shared" si="3"/>
+        <v>22.459018333333333</v>
+      </c>
+      <c r="AC52" s="41">
+        <v>701</v>
+      </c>
+      <c r="AD52">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:30" ht="15" thickBot="1">
       <c r="A53">
         <v>1972</v>
       </c>
@@ -4941,11 +5731,25 @@
         <v>158</v>
       </c>
       <c r="Y53">
+        <f t="shared" si="4"/>
+        <v>466</v>
+      </c>
+      <c r="AA53">
         <f t="shared" si="2"/>
-        <v>466</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" ht="15" thickBot="1">
+        <v>9.1570566666666657</v>
+      </c>
+      <c r="AB53">
+        <f t="shared" si="3"/>
+        <v>20.917056666666667</v>
+      </c>
+      <c r="AC53" s="41">
+        <v>716</v>
+      </c>
+      <c r="AD53">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" ht="15" thickBot="1">
       <c r="A54">
         <v>1973</v>
       </c>
@@ -5018,11 +5822,25 @@
         <v>123</v>
       </c>
       <c r="Y54">
+        <f t="shared" si="4"/>
+        <v>356</v>
+      </c>
+      <c r="AA54">
         <f t="shared" si="2"/>
-        <v>356</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" ht="15" thickBot="1">
+        <v>10.455468333333332</v>
+      </c>
+      <c r="AB54">
+        <f t="shared" si="3"/>
+        <v>21.975468333333332</v>
+      </c>
+      <c r="AC54" s="41">
+        <v>707</v>
+      </c>
+      <c r="AD54">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" ht="15" thickBot="1">
       <c r="A55">
         <v>1974</v>
       </c>
@@ -5095,11 +5913,25 @@
         <v>185</v>
       </c>
       <c r="Y55">
+        <f t="shared" si="4"/>
+        <v>504</v>
+      </c>
+      <c r="AA55">
         <f t="shared" si="2"/>
-        <v>504</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" ht="15" thickBot="1">
+        <v>9.9109300000000005</v>
+      </c>
+      <c r="AB55">
+        <f t="shared" si="3"/>
+        <v>21.190930000000002</v>
+      </c>
+      <c r="AC55" s="41">
+        <v>609</v>
+      </c>
+      <c r="AD55">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:30" ht="15" thickBot="1">
       <c r="A56">
         <v>1975</v>
       </c>
@@ -5172,11 +6004,25 @@
         <v>171</v>
       </c>
       <c r="Y56">
+        <f t="shared" si="4"/>
+        <v>502</v>
+      </c>
+      <c r="AA56">
         <f t="shared" si="2"/>
-        <v>502</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25" ht="15" thickBot="1">
+        <v>10.364679999999998</v>
+      </c>
+      <c r="AB56">
+        <f t="shared" si="3"/>
+        <v>21.404679999999999</v>
+      </c>
+      <c r="AC56" s="41">
+        <v>802</v>
+      </c>
+      <c r="AD56">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30" ht="15" thickBot="1">
       <c r="A57">
         <v>1976</v>
       </c>
@@ -5249,11 +6095,25 @@
         <v>247</v>
       </c>
       <c r="Y57">
+        <f t="shared" si="4"/>
+        <v>380</v>
+      </c>
+      <c r="AA57">
         <f t="shared" si="2"/>
-        <v>380</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" ht="15" thickBot="1">
+        <v>10.352765000000002</v>
+      </c>
+      <c r="AB57">
+        <f t="shared" si="3"/>
+        <v>21.152764999999999</v>
+      </c>
+      <c r="AC57" s="41">
+        <v>782</v>
+      </c>
+      <c r="AD57">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30" ht="15" thickBot="1">
       <c r="A58">
         <v>1977</v>
       </c>
@@ -5326,11 +6186,25 @@
         <v>87</v>
       </c>
       <c r="Y58">
+        <f t="shared" si="4"/>
+        <v>755</v>
+      </c>
+      <c r="AA58">
         <f t="shared" si="2"/>
-        <v>755</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" ht="15" thickBot="1">
+        <v>10.140836666666663</v>
+      </c>
+      <c r="AB58">
+        <f t="shared" si="3"/>
+        <v>20.700836666666664</v>
+      </c>
+      <c r="AC58" s="41">
+        <v>712</v>
+      </c>
+      <c r="AD58">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" ht="15" thickBot="1">
       <c r="A59">
         <v>1978</v>
       </c>
@@ -5403,11 +6277,25 @@
         <v>51</v>
       </c>
       <c r="Y59">
+        <f t="shared" si="4"/>
+        <v>622</v>
+      </c>
+      <c r="AA59">
         <f t="shared" si="2"/>
-        <v>622</v>
-      </c>
-    </row>
-    <row r="60" spans="1:25" ht="15" thickBot="1">
+        <v>10.271143333333335</v>
+      </c>
+      <c r="AB59">
+        <f t="shared" si="3"/>
+        <v>20.591143333333335</v>
+      </c>
+      <c r="AC59" s="41">
+        <v>707</v>
+      </c>
+      <c r="AD59">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30" ht="15" thickBot="1">
       <c r="A60">
         <v>1979</v>
       </c>
@@ -5480,11 +6368,25 @@
         <v>122</v>
       </c>
       <c r="Y60">
+        <f t="shared" si="4"/>
+        <v>602</v>
+      </c>
+      <c r="AA60">
         <f t="shared" si="2"/>
-        <v>602</v>
-      </c>
-    </row>
-    <row r="61" spans="1:25" ht="15" thickBot="1">
+        <v>10.190378333333335</v>
+      </c>
+      <c r="AB60">
+        <f t="shared" si="3"/>
+        <v>20.270378333333337</v>
+      </c>
+      <c r="AC60" s="41">
+        <v>753</v>
+      </c>
+      <c r="AD60">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:30" ht="15" thickBot="1">
       <c r="A61">
         <v>1980</v>
       </c>
@@ -5557,11 +6459,25 @@
         <v>74</v>
       </c>
       <c r="Y61">
+        <f t="shared" si="4"/>
+        <v>552</v>
+      </c>
+      <c r="AA61">
         <f t="shared" si="2"/>
-        <v>552</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25" ht="15" thickBot="1">
+        <v>10.22236</v>
+      </c>
+      <c r="AB61">
+        <f t="shared" si="3"/>
+        <v>20.062359999999998</v>
+      </c>
+      <c r="AC61" s="41">
+        <v>741</v>
+      </c>
+      <c r="AD61">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" ht="15" thickBot="1">
       <c r="A62">
         <v>1981</v>
       </c>
@@ -5634,11 +6550,25 @@
         <v>111</v>
       </c>
       <c r="Y62">
+        <f t="shared" si="4"/>
+        <v>498</v>
+      </c>
+      <c r="AA62">
         <f t="shared" si="2"/>
-        <v>498</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25" ht="15" thickBot="1">
+        <v>10.604333333333335</v>
+      </c>
+      <c r="AB62">
+        <f t="shared" si="3"/>
+        <v>20.204333333333334</v>
+      </c>
+      <c r="AC62" s="41">
+        <v>878</v>
+      </c>
+      <c r="AD62">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:30" ht="15" thickBot="1">
       <c r="A63">
         <v>1982</v>
       </c>
@@ -5711,11 +6641,25 @@
         <v>162</v>
       </c>
       <c r="Y63">
+        <f t="shared" si="4"/>
+        <v>709</v>
+      </c>
+      <c r="AA63">
         <f t="shared" si="2"/>
-        <v>709</v>
-      </c>
-    </row>
-    <row r="64" spans="1:25" ht="15" thickBot="1">
+        <v>10.920475</v>
+      </c>
+      <c r="AB63">
+        <f t="shared" si="3"/>
+        <v>20.280474999999999</v>
+      </c>
+      <c r="AC63" s="41">
+        <v>4193</v>
+      </c>
+      <c r="AD63">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:30" ht="15" thickBot="1">
       <c r="A64">
         <v>1983</v>
       </c>
@@ -5788,11 +6732,25 @@
         <v>119</v>
       </c>
       <c r="Y64">
+        <f t="shared" si="4"/>
+        <v>699</v>
+      </c>
+      <c r="AA64">
         <f t="shared" si="2"/>
-        <v>699</v>
-      </c>
-    </row>
-    <row r="65" spans="1:25" ht="15" thickBot="1">
+        <v>11.057651666666665</v>
+      </c>
+      <c r="AB64">
+        <f t="shared" si="3"/>
+        <v>20.177651666666662</v>
+      </c>
+      <c r="AC64" s="41">
+        <v>837</v>
+      </c>
+      <c r="AD64">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:30" ht="15" thickBot="1">
       <c r="A65">
         <v>1984</v>
       </c>
@@ -5865,11 +6823,25 @@
         <v>145</v>
       </c>
       <c r="Y65">
+        <f t="shared" si="4"/>
+        <v>573</v>
+      </c>
+      <c r="AA65">
         <f t="shared" si="2"/>
-        <v>573</v>
-      </c>
-    </row>
-    <row r="66" spans="1:25" ht="15" thickBot="1">
+        <v>10.252216666666669</v>
+      </c>
+      <c r="AB65">
+        <f t="shared" si="3"/>
+        <v>19.132216666666668</v>
+      </c>
+      <c r="AC65" s="41">
+        <v>715</v>
+      </c>
+      <c r="AD65">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="66" spans="1:30" ht="15" thickBot="1">
       <c r="A66">
         <v>1985</v>
       </c>
@@ -5942,11 +6914,25 @@
         <v>38</v>
       </c>
       <c r="Y66">
+        <f t="shared" si="4"/>
+        <v>668</v>
+      </c>
+      <c r="AA66">
         <f t="shared" si="2"/>
-        <v>668</v>
-      </c>
-    </row>
-    <row r="67" spans="1:25" ht="15" thickBot="1">
+        <v>10.982785</v>
+      </c>
+      <c r="AB66">
+        <f t="shared" si="3"/>
+        <v>19.622784999999997</v>
+      </c>
+      <c r="AC66" s="41">
+        <v>833</v>
+      </c>
+      <c r="AD66">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:30" ht="15" thickBot="1">
       <c r="A67">
         <v>1986</v>
       </c>
@@ -5972,7 +6958,7 @@
         <v>14.9</v>
       </c>
       <c r="I67" s="9">
-        <f t="shared" ref="I67:I102" si="3">SUM(B67:G67)/6</f>
+        <f t="shared" ref="I67:I102" si="5">SUM(B67:G67)/6</f>
         <v>16.283333333333335</v>
       </c>
       <c r="K67" s="28">
@@ -6015,15 +7001,29 @@
         <v>954</v>
       </c>
       <c r="X67">
-        <f t="shared" ref="X67:X102" si="4">SUM(R67:S67)</f>
+        <f t="shared" ref="X67:X102" si="6">SUM(R67:S67)</f>
         <v>171</v>
       </c>
       <c r="Y67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>519</v>
       </c>
-    </row>
-    <row r="68" spans="1:25" ht="15" thickBot="1">
+      <c r="AA67">
+        <f t="shared" ref="AA67:AA102" si="7">0.608*I67-0.0038*X67+0.00115*Y67+0.00765*G67</f>
+        <v>9.9811916666666658</v>
+      </c>
+      <c r="AB67">
+        <f t="shared" ref="AB67:AB102" si="8">0.24*(2021-A67)+0.608*I67-0.0038*X67+0.00115*Y67+0.00765*G67</f>
+        <v>18.381191666666666</v>
+      </c>
+      <c r="AC67" s="41">
+        <v>1427</v>
+      </c>
+      <c r="AD67">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:30" ht="15" thickBot="1">
       <c r="A68">
         <v>1987</v>
       </c>
@@ -6049,7 +7049,7 @@
         <v>14.2</v>
       </c>
       <c r="I68" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.433333333333334</v>
       </c>
       <c r="K68" s="11">
@@ -6092,15 +7092,29 @@
         <v>788</v>
       </c>
       <c r="X68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>115</v>
       </c>
       <c r="Y68">
-        <f t="shared" ref="Y68:Y102" si="5">SUM(K68:M68)+SUM(T67:V67)</f>
+        <f t="shared" ref="Y68:Y102" si="9">SUM(K68:M68)+SUM(T67:V67)</f>
         <v>398</v>
       </c>
-    </row>
-    <row r="69" spans="1:25" ht="15" thickBot="1">
+      <c r="AA68">
+        <f t="shared" si="7"/>
+        <v>10.771636666666666</v>
+      </c>
+      <c r="AB68">
+        <f t="shared" si="8"/>
+        <v>18.931636666666666</v>
+      </c>
+      <c r="AC68" s="41">
+        <v>705</v>
+      </c>
+      <c r="AD68">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" ht="15" thickBot="1">
       <c r="A69">
         <v>1988</v>
       </c>
@@ -6126,7 +7140,7 @@
         <v>14.9</v>
       </c>
       <c r="I69" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.25</v>
       </c>
       <c r="K69" s="34">
@@ -6169,15 +7183,29 @@
         <v>943</v>
       </c>
       <c r="X69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>59</v>
       </c>
       <c r="Y69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>735</v>
       </c>
-    </row>
-    <row r="70" spans="1:25" ht="15" thickBot="1">
+      <c r="AA69">
+        <f t="shared" si="7"/>
+        <v>11.242925</v>
+      </c>
+      <c r="AB69">
+        <f t="shared" si="8"/>
+        <v>19.162925000000001</v>
+      </c>
+      <c r="AC69" s="41">
+        <v>999</v>
+      </c>
+      <c r="AD69">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="70" spans="1:30" ht="15" thickBot="1">
       <c r="A70">
         <v>1989</v>
       </c>
@@ -6203,7 +7231,7 @@
         <v>15</v>
       </c>
       <c r="I70" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.45</v>
       </c>
       <c r="K70" s="11">
@@ -6246,15 +7274,29 @@
         <v>668</v>
       </c>
       <c r="X70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>86</v>
       </c>
       <c r="Y70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>283</v>
       </c>
-    </row>
-    <row r="71" spans="1:25" ht="15" thickBot="1">
+      <c r="AA70">
+        <f t="shared" si="7"/>
+        <v>11.355479999999998</v>
+      </c>
+      <c r="AB70">
+        <f t="shared" si="8"/>
+        <v>19.03548</v>
+      </c>
+      <c r="AC70" s="41">
+        <v>885</v>
+      </c>
+      <c r="AD70">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" ht="15" thickBot="1">
       <c r="A71">
         <v>1990</v>
       </c>
@@ -6280,7 +7322,7 @@
         <v>15.1</v>
       </c>
       <c r="I71" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.566666666666666</v>
       </c>
       <c r="K71" s="10">
@@ -6323,15 +7365,29 @@
         <v>906</v>
       </c>
       <c r="X71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="Y71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>380</v>
       </c>
-    </row>
-    <row r="72" spans="1:25" ht="15" thickBot="1">
+      <c r="AA71">
+        <f t="shared" si="7"/>
+        <v>11.566883333333333</v>
+      </c>
+      <c r="AB71">
+        <f t="shared" si="8"/>
+        <v>19.006883333333334</v>
+      </c>
+      <c r="AC71" s="41">
+        <v>1111</v>
+      </c>
+      <c r="AD71">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" ht="15" thickBot="1">
       <c r="A72">
         <v>1991</v>
       </c>
@@ -6357,7 +7413,7 @@
         <v>12.2</v>
       </c>
       <c r="I72" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.7</v>
       </c>
       <c r="K72" s="12">
@@ -6400,15 +7456,29 @@
         <v>978</v>
       </c>
       <c r="X72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>182</v>
       </c>
       <c r="Y72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>519</v>
       </c>
-    </row>
-    <row r="73" spans="1:25" ht="15" thickBot="1">
+      <c r="AA72">
+        <f t="shared" si="7"/>
+        <v>10.82138</v>
+      </c>
+      <c r="AB72">
+        <f t="shared" si="8"/>
+        <v>18.021379999999997</v>
+      </c>
+      <c r="AC72" s="41">
+        <v>766</v>
+      </c>
+      <c r="AD72">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:30" ht="15" thickBot="1">
       <c r="A73">
         <v>1992</v>
       </c>
@@ -6434,7 +7504,7 @@
         <v>11.7</v>
       </c>
       <c r="I73" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.583333333333332</v>
       </c>
       <c r="K73" s="11">
@@ -6477,15 +7547,29 @@
         <v>1231</v>
       </c>
       <c r="X73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>342</v>
       </c>
       <c r="Y73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>488</v>
       </c>
-    </row>
-    <row r="74" spans="1:25" ht="15" thickBot="1">
+      <c r="AA73">
+        <f t="shared" si="7"/>
+        <v>10.080786666666665</v>
+      </c>
+      <c r="AB73">
+        <f t="shared" si="8"/>
+        <v>17.040786666666666</v>
+      </c>
+      <c r="AC73" s="41">
+        <v>746</v>
+      </c>
+      <c r="AD73">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:30" ht="15" thickBot="1">
       <c r="A74">
         <v>1993</v>
       </c>
@@ -6511,7 +7595,7 @@
         <v>12.3</v>
       </c>
       <c r="I74" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.099999999999998</v>
       </c>
       <c r="K74" s="17">
@@ -6554,15 +7638,29 @@
         <v>1089</v>
       </c>
       <c r="X74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>278</v>
       </c>
       <c r="Y74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>446</v>
       </c>
-    </row>
-    <row r="75" spans="1:25" ht="15" thickBot="1">
+      <c r="AA74">
+        <f t="shared" si="7"/>
+        <v>9.9764649999999993</v>
+      </c>
+      <c r="AB74">
+        <f t="shared" si="8"/>
+        <v>16.696464999999996</v>
+      </c>
+      <c r="AC74" s="41">
+        <v>701</v>
+      </c>
+      <c r="AD74">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:30" ht="15" thickBot="1">
       <c r="A75">
         <v>1994</v>
       </c>
@@ -6588,7 +7686,7 @@
         <v>14.6</v>
       </c>
       <c r="I75" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.816666666666666</v>
       </c>
       <c r="K75" s="29">
@@ -6631,15 +7729,29 @@
         <v>1156</v>
       </c>
       <c r="X75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>220</v>
       </c>
       <c r="Y75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>709</v>
       </c>
-    </row>
-    <row r="76" spans="1:25" ht="15" thickBot="1">
+      <c r="AA75">
+        <f t="shared" si="7"/>
+        <v>10.937343333333333</v>
+      </c>
+      <c r="AB75">
+        <f t="shared" si="8"/>
+        <v>17.417343333333331</v>
+      </c>
+      <c r="AC75" s="41">
+        <v>883</v>
+      </c>
+      <c r="AD75">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="76" spans="1:30" ht="15" thickBot="1">
       <c r="A76">
         <v>1995</v>
       </c>
@@ -6665,7 +7777,7 @@
         <v>17</v>
       </c>
       <c r="I76" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.083333333333332</v>
       </c>
       <c r="K76" s="20">
@@ -6708,15 +7820,29 @@
         <v>1048</v>
       </c>
       <c r="X76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>171</v>
       </c>
       <c r="Y76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>568</v>
       </c>
-    </row>
-    <row r="77" spans="1:25" ht="15" thickBot="1">
+      <c r="AA76">
+        <f t="shared" si="7"/>
+        <v>11.121231666666665</v>
+      </c>
+      <c r="AB76">
+        <f t="shared" si="8"/>
+        <v>17.361231666666669</v>
+      </c>
+      <c r="AC76" s="41">
+        <v>967</v>
+      </c>
+      <c r="AD76">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:30" ht="15" thickBot="1">
       <c r="A77">
         <v>1996</v>
       </c>
@@ -6742,7 +7868,7 @@
         <v>13.7</v>
       </c>
       <c r="I77" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.516666666666666</v>
       </c>
       <c r="K77" s="15">
@@ -6785,15 +7911,29 @@
         <v>1106</v>
       </c>
       <c r="X77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>254</v>
       </c>
       <c r="Y77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>636</v>
       </c>
-    </row>
-    <row r="78" spans="1:25" ht="15" thickBot="1">
+      <c r="AA77">
+        <f t="shared" si="7"/>
+        <v>10.541028333333333</v>
+      </c>
+      <c r="AB77">
+        <f t="shared" si="8"/>
+        <v>16.541028333333333</v>
+      </c>
+      <c r="AC77" s="41">
+        <v>1215</v>
+      </c>
+      <c r="AD77">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:30" ht="15" thickBot="1">
       <c r="A78">
         <v>1997</v>
       </c>
@@ -6819,7 +7959,7 @@
         <v>15.4</v>
       </c>
       <c r="I78" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.8</v>
       </c>
       <c r="K78" s="12">
@@ -6862,15 +8002,29 @@
         <v>1106</v>
       </c>
       <c r="X78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>112</v>
       </c>
       <c r="Y78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>460</v>
       </c>
-    </row>
-    <row r="79" spans="1:25" ht="15" thickBot="1">
+      <c r="AA78">
+        <f t="shared" si="7"/>
+        <v>11.682975000000001</v>
+      </c>
+      <c r="AB78">
+        <f t="shared" si="8"/>
+        <v>17.442975000000001</v>
+      </c>
+      <c r="AC78" s="41">
+        <v>760</v>
+      </c>
+      <c r="AD78">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:30" ht="15" thickBot="1">
       <c r="A79">
         <v>1998</v>
       </c>
@@ -6896,7 +8050,7 @@
         <v>13.5</v>
       </c>
       <c r="I79" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.816666666666666</v>
       </c>
       <c r="K79" s="21">
@@ -6939,15 +8093,29 @@
         <v>1011</v>
       </c>
       <c r="X79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>197</v>
       </c>
       <c r="Y79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>693</v>
       </c>
-    </row>
-    <row r="80" spans="1:25" ht="15" thickBot="1">
+      <c r="AA79">
+        <f t="shared" si="7"/>
+        <v>11.020113333333333</v>
+      </c>
+      <c r="AB79">
+        <f t="shared" si="8"/>
+        <v>16.540113333333334</v>
+      </c>
+      <c r="AC79" s="41">
+        <v>985</v>
+      </c>
+      <c r="AD79">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:30" ht="15" thickBot="1">
       <c r="A80">
         <v>1999</v>
       </c>
@@ -6973,7 +8141,7 @@
         <v>14.6</v>
       </c>
       <c r="I80" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.650000000000002</v>
       </c>
       <c r="K80" s="10">
@@ -7016,15 +8184,29 @@
         <v>1100</v>
       </c>
       <c r="X80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>254</v>
       </c>
       <c r="Y80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>501</v>
       </c>
-    </row>
-    <row r="81" spans="1:25" ht="15" thickBot="1">
+      <c r="AA80">
+        <f t="shared" si="7"/>
+        <v>11.099325000000002</v>
+      </c>
+      <c r="AB80">
+        <f t="shared" si="8"/>
+        <v>16.379324999999998</v>
+      </c>
+      <c r="AC80" s="41">
+        <v>945</v>
+      </c>
+      <c r="AD80">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="81" spans="1:30" ht="15" thickBot="1">
       <c r="A81">
         <v>2000</v>
       </c>
@@ -7050,7 +8232,7 @@
         <v>14.1</v>
       </c>
       <c r="I81" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.299999999999997</v>
       </c>
       <c r="K81" s="16">
@@ -7093,15 +8275,29 @@
         <v>1209</v>
       </c>
       <c r="X81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>69</v>
       </c>
       <c r="Y81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>488</v>
       </c>
-    </row>
-    <row r="82" spans="1:25" ht="15" thickBot="1">
+      <c r="AA81">
+        <f t="shared" si="7"/>
+        <v>11.569984999999997</v>
+      </c>
+      <c r="AB81">
+        <f t="shared" si="8"/>
+        <v>16.609984999999998</v>
+      </c>
+      <c r="AC81" s="41">
+        <v>1703</v>
+      </c>
+      <c r="AD81">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:30" ht="15" thickBot="1">
       <c r="A82">
         <v>2001</v>
       </c>
@@ -7127,7 +8323,7 @@
         <v>16.8</v>
       </c>
       <c r="I82" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.766666666666666</v>
       </c>
       <c r="K82" s="20">
@@ -7170,15 +8366,29 @@
         <v>807</v>
       </c>
       <c r="X82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="Y82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>926</v>
       </c>
-    </row>
-    <row r="83" spans="1:25" ht="15" thickBot="1">
+      <c r="AA82">
+        <f t="shared" si="7"/>
+        <v>11.651258333333331</v>
+      </c>
+      <c r="AB82">
+        <f t="shared" si="8"/>
+        <v>16.451258333333332</v>
+      </c>
+      <c r="AC82" s="41">
+        <v>1001</v>
+      </c>
+      <c r="AD82">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:30" ht="15" thickBot="1">
       <c r="A83">
         <v>2002</v>
       </c>
@@ -7204,7 +8414,7 @@
         <v>15</v>
       </c>
       <c r="I83" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.3</v>
       </c>
       <c r="K83" s="16">
@@ -7247,15 +8457,29 @@
         <v>723</v>
       </c>
       <c r="X83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>143</v>
       </c>
       <c r="Y83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>277</v>
       </c>
-    </row>
-    <row r="84" spans="1:25" ht="15" thickBot="1">
+      <c r="AA83">
+        <f t="shared" si="7"/>
+        <v>10.428955</v>
+      </c>
+      <c r="AB83">
+        <f t="shared" si="8"/>
+        <v>14.988954999999999</v>
+      </c>
+      <c r="AC83" s="41">
+        <v>832</v>
+      </c>
+      <c r="AD83">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="84" spans="1:30" ht="15" thickBot="1">
       <c r="A84">
         <v>2003</v>
       </c>
@@ -7281,7 +8505,7 @@
         <v>12.9</v>
       </c>
       <c r="I84" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19.833333333333332</v>
       </c>
       <c r="K84" s="19">
@@ -7324,15 +8548,29 @@
         <v>735</v>
       </c>
       <c r="X84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
       <c r="Y84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>461</v>
       </c>
-    </row>
-    <row r="85" spans="1:25" ht="15" thickBot="1">
+      <c r="AA84">
+        <f t="shared" si="7"/>
+        <v>12.475766666666667</v>
+      </c>
+      <c r="AB84">
+        <f t="shared" si="8"/>
+        <v>16.795766666666665</v>
+      </c>
+      <c r="AC84" s="41">
+        <v>1171</v>
+      </c>
+      <c r="AD84">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="85" spans="1:30" ht="15" thickBot="1">
       <c r="A85">
         <v>2004</v>
       </c>
@@ -7358,7 +8596,7 @@
         <v>15.4</v>
       </c>
       <c r="I85" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.116666666666667</v>
       </c>
       <c r="K85" s="25">
@@ -7401,15 +8639,29 @@
         <v>695</v>
       </c>
       <c r="X85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>122</v>
       </c>
       <c r="Y85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>487</v>
       </c>
-    </row>
-    <row r="86" spans="1:25" ht="15" thickBot="1">
+      <c r="AA85">
+        <f t="shared" si="7"/>
+        <v>11.256733333333335</v>
+      </c>
+      <c r="AB85">
+        <f t="shared" si="8"/>
+        <v>15.336733333333335</v>
+      </c>
+      <c r="AC85" s="41">
+        <v>911</v>
+      </c>
+      <c r="AD85">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:30" ht="15" thickBot="1">
       <c r="A86">
         <v>2005</v>
       </c>
@@ -7435,7 +8687,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="I86" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.683333333333334</v>
       </c>
       <c r="K86" s="11">
@@ -7478,15 +8730,29 @@
         <v>593</v>
       </c>
       <c r="X86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="Y86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>284</v>
       </c>
-    </row>
-    <row r="87" spans="1:25" ht="15" thickBot="1">
+      <c r="AA86">
+        <f t="shared" si="7"/>
+        <v>11.557766666666668</v>
+      </c>
+      <c r="AB86">
+        <f t="shared" si="8"/>
+        <v>15.397766666666667</v>
+      </c>
+      <c r="AC86" s="41">
+        <v>1106</v>
+      </c>
+      <c r="AD86">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:30" ht="15" thickBot="1">
       <c r="A87">
         <v>2006</v>
       </c>
@@ -7512,7 +8778,7 @@
         <v>17.2</v>
       </c>
       <c r="I87" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19.116666666666664</v>
       </c>
       <c r="K87" s="18">
@@ -7555,15 +8821,29 @@
         <v>821</v>
       </c>
       <c r="X87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>170</v>
       </c>
       <c r="Y87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>591</v>
       </c>
-    </row>
-    <row r="88" spans="1:25" ht="15" thickBot="1">
+      <c r="AA87">
+        <f t="shared" si="7"/>
+        <v>11.81340833333333</v>
+      </c>
+      <c r="AB87">
+        <f t="shared" si="8"/>
+        <v>15.413408333333329</v>
+      </c>
+      <c r="AC87" s="41">
+        <v>978</v>
+      </c>
+      <c r="AD87">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:30" ht="15" thickBot="1">
       <c r="A88">
         <v>2007</v>
       </c>
@@ -7589,7 +8869,7 @@
         <v>13.4</v>
       </c>
       <c r="I88" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.849999999999998</v>
       </c>
       <c r="K88" s="24">
@@ -7632,15 +8912,29 @@
         <v>881</v>
       </c>
       <c r="X88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>121</v>
       </c>
       <c r="Y88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>486</v>
       </c>
-    </row>
-    <row r="89" spans="1:25" ht="15" thickBot="1">
+      <c r="AA88">
+        <f t="shared" si="7"/>
+        <v>11.082714999999999</v>
+      </c>
+      <c r="AB88">
+        <f t="shared" si="8"/>
+        <v>14.442714999999998</v>
+      </c>
+      <c r="AC88" s="41">
+        <v>952</v>
+      </c>
+      <c r="AD88">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="89" spans="1:30" ht="15" thickBot="1">
       <c r="A89">
         <v>2008</v>
       </c>
@@ -7666,7 +8960,7 @@
         <v>13</v>
       </c>
       <c r="I89" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.299999999999997</v>
       </c>
       <c r="K89" s="21">
@@ -7709,15 +9003,29 @@
         <v>1012</v>
       </c>
       <c r="X89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>149</v>
       </c>
       <c r="Y89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>399</v>
       </c>
-    </row>
-    <row r="90" spans="1:25" ht="15" thickBot="1">
+      <c r="AA89">
+        <f t="shared" si="7"/>
+        <v>10.537274999999998</v>
+      </c>
+      <c r="AB89">
+        <f t="shared" si="8"/>
+        <v>13.657274999999997</v>
+      </c>
+      <c r="AC89" s="41">
+        <v>1167</v>
+      </c>
+      <c r="AD89">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="90" spans="1:30" ht="15" thickBot="1">
       <c r="A90">
         <v>2009</v>
       </c>
@@ -7743,7 +9051,7 @@
         <v>15</v>
       </c>
       <c r="I90" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.433333333333334</v>
       </c>
       <c r="K90" s="20">
@@ -7786,15 +9094,29 @@
         <v>912</v>
       </c>
       <c r="X90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>73</v>
       </c>
       <c r="Y90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>488</v>
       </c>
-    </row>
-    <row r="91" spans="1:25" ht="15" thickBot="1">
+      <c r="AA90">
+        <f t="shared" si="7"/>
+        <v>11.634321666666667</v>
+      </c>
+      <c r="AB90">
+        <f t="shared" si="8"/>
+        <v>14.514321666666667</v>
+      </c>
+      <c r="AC90" s="41">
+        <v>1172</v>
+      </c>
+      <c r="AD90">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="91" spans="1:30" ht="15" thickBot="1">
       <c r="A91">
         <v>2010</v>
       </c>
@@ -7820,7 +9142,7 @@
         <v>13.5</v>
       </c>
       <c r="I91" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.05</v>
       </c>
       <c r="K91" s="24">
@@ -7863,15 +9185,29 @@
         <v>814</v>
       </c>
       <c r="X91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>41</v>
       </c>
       <c r="Y91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>530</v>
       </c>
-    </row>
-    <row r="92" spans="1:25" ht="15" thickBot="1">
+      <c r="AA91">
+        <f t="shared" si="7"/>
+        <v>11.565035000000002</v>
+      </c>
+      <c r="AB91">
+        <f t="shared" si="8"/>
+        <v>14.205035000000001</v>
+      </c>
+      <c r="AC91" s="41">
+        <v>1240</v>
+      </c>
+      <c r="AD91">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="92" spans="1:30" ht="15" thickBot="1">
       <c r="A92">
         <v>2011</v>
       </c>
@@ -7897,7 +9233,7 @@
         <v>14.8</v>
       </c>
       <c r="I92" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="K92" s="11">
@@ -7940,15 +9276,29 @@
         <v>588</v>
       </c>
       <c r="X92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>114</v>
       </c>
       <c r="Y92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>511</v>
       </c>
-    </row>
-    <row r="93" spans="1:25" ht="15" thickBot="1">
+      <c r="AA92">
+        <f t="shared" si="7"/>
+        <v>11.856390000000001</v>
+      </c>
+      <c r="AB92">
+        <f t="shared" si="8"/>
+        <v>14.256390000000001</v>
+      </c>
+      <c r="AC92" s="41">
+        <v>875</v>
+      </c>
+      <c r="AD92">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="93" spans="1:30" ht="15" thickBot="1">
       <c r="A93">
         <v>2012</v>
       </c>
@@ -7974,7 +9324,7 @@
         <v>14.5</v>
       </c>
       <c r="I93" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.983333333333331</v>
       </c>
       <c r="K93" s="18">
@@ -8017,15 +9367,29 @@
         <v>847</v>
       </c>
       <c r="X93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>78</v>
       </c>
       <c r="Y93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>341</v>
       </c>
-    </row>
-    <row r="94" spans="1:25" ht="15" thickBot="1">
+      <c r="AA93">
+        <f t="shared" si="7"/>
+        <v>11.172671666666666</v>
+      </c>
+      <c r="AB93">
+        <f t="shared" si="8"/>
+        <v>13.332671666666666</v>
+      </c>
+      <c r="AC93" s="41">
+        <v>792</v>
+      </c>
+      <c r="AD93">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:30" ht="15" thickBot="1">
       <c r="A94">
         <v>2013</v>
       </c>
@@ -8051,7 +9415,7 @@
         <v>15.9</v>
       </c>
       <c r="I94" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.650000000000002</v>
       </c>
       <c r="K94" s="25">
@@ -8094,15 +9458,29 @@
         <v>1050</v>
       </c>
       <c r="X94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>132</v>
       </c>
       <c r="Y94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>646</v>
       </c>
-    </row>
-    <row r="95" spans="1:25" ht="15" thickBot="1">
+      <c r="AA94">
+        <f t="shared" si="7"/>
+        <v>11.114025000000002</v>
+      </c>
+      <c r="AB94">
+        <f t="shared" si="8"/>
+        <v>13.034025000000002</v>
+      </c>
+      <c r="AC94" s="41">
+        <v>909</v>
+      </c>
+      <c r="AD94">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:30" ht="15" thickBot="1">
       <c r="A95">
         <v>2014</v>
       </c>
@@ -8128,7 +9506,7 @@
         <v>16.7</v>
       </c>
       <c r="I95" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.3</v>
       </c>
       <c r="K95" s="29">
@@ -8171,15 +9549,29 @@
         <v>1001</v>
       </c>
       <c r="X95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>102</v>
       </c>
       <c r="Y95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>674</v>
       </c>
-    </row>
-    <row r="96" spans="1:25" ht="15" thickBot="1">
+      <c r="AA95">
+        <f t="shared" si="7"/>
+        <v>11.668429999999999</v>
+      </c>
+      <c r="AB95">
+        <f t="shared" si="8"/>
+        <v>13.348429999999999</v>
+      </c>
+      <c r="AC95" s="41">
+        <v>846</v>
+      </c>
+      <c r="AD95">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:30" ht="15" thickBot="1">
       <c r="A96">
         <v>2015</v>
       </c>
@@ -8205,7 +9597,7 @@
         <v>13.3</v>
       </c>
       <c r="I96" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.7</v>
       </c>
       <c r="K96" s="19">
@@ -8248,15 +9640,29 @@
         <v>596</v>
       </c>
       <c r="X96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>125</v>
       </c>
       <c r="Y96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>439</v>
       </c>
-    </row>
-    <row r="97" spans="1:25" ht="15" thickBot="1">
+      <c r="AA96">
+        <f t="shared" si="7"/>
+        <v>11.529500000000001</v>
+      </c>
+      <c r="AB96">
+        <f t="shared" si="8"/>
+        <v>12.9695</v>
+      </c>
+      <c r="AC96" s="41">
+        <v>898</v>
+      </c>
+      <c r="AD96">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:30" ht="15" thickBot="1">
       <c r="A97">
         <v>2016</v>
       </c>
@@ -8282,7 +9688,7 @@
         <v>13.3</v>
       </c>
       <c r="I97" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.366666666666667</v>
       </c>
       <c r="K97" s="34">
@@ -8325,15 +9731,29 @@
         <v>924</v>
       </c>
       <c r="X97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
       <c r="Y97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>613</v>
       </c>
-    </row>
-    <row r="98" spans="1:25" ht="15" thickBot="1">
+      <c r="AA97">
+        <f t="shared" si="7"/>
+        <v>11.737613333333332</v>
+      </c>
+      <c r="AB97">
+        <f t="shared" si="8"/>
+        <v>12.937613333333331</v>
+      </c>
+      <c r="AC97" s="41">
+        <v>1015</v>
+      </c>
+      <c r="AD97">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="98" spans="1:30" ht="15" thickBot="1">
       <c r="A98">
         <v>2017</v>
       </c>
@@ -8359,7 +9779,7 @@
         <v>15.6</v>
       </c>
       <c r="I98" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.599999999999998</v>
       </c>
       <c r="K98" s="11">
@@ -8402,15 +9822,29 @@
         <v>762</v>
       </c>
       <c r="X98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>102</v>
       </c>
       <c r="Y98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>279</v>
       </c>
-    </row>
-    <row r="99" spans="1:25" ht="15" thickBot="1">
+      <c r="AA98">
+        <f t="shared" si="7"/>
+        <v>11.370569999999997</v>
+      </c>
+      <c r="AB98">
+        <f t="shared" si="8"/>
+        <v>12.330569999999998</v>
+      </c>
+      <c r="AC98" s="41">
+        <v>866</v>
+      </c>
+      <c r="AD98">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:30" ht="15" thickBot="1">
       <c r="A99">
         <v>2018</v>
       </c>
@@ -8436,7 +9870,7 @@
         <v>14.4</v>
       </c>
       <c r="I99" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19.549999999999997</v>
       </c>
       <c r="K99" s="23">
@@ -8479,15 +9913,29 @@
         <v>579</v>
       </c>
       <c r="X99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="Y99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>526</v>
       </c>
-    </row>
-    <row r="100" spans="1:25" ht="15" thickBot="1">
+      <c r="AA99">
+        <f t="shared" si="7"/>
+        <v>12.559934999999998</v>
+      </c>
+      <c r="AB99">
+        <f t="shared" si="8"/>
+        <v>13.279934999999998</v>
+      </c>
+      <c r="AC99" s="41">
+        <v>1072</v>
+      </c>
+      <c r="AD99">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:30" ht="15" thickBot="1">
       <c r="A100">
         <v>2019</v>
       </c>
@@ -8513,7 +9961,7 @@
         <v>16</v>
       </c>
       <c r="I100" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.633333333333333</v>
       </c>
       <c r="K100" s="17">
@@ -8556,15 +10004,29 @@
         <v>549</v>
       </c>
       <c r="X100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>54</v>
       </c>
       <c r="Y100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="101" spans="1:25" ht="15" thickBot="1">
+      <c r="AA100">
+        <f t="shared" si="7"/>
+        <v>11.346261666666667</v>
+      </c>
+      <c r="AB100">
+        <f t="shared" si="8"/>
+        <v>11.826261666666667</v>
+      </c>
+      <c r="AC100" s="41">
+        <v>912</v>
+      </c>
+      <c r="AD100">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:30" ht="15" thickBot="1">
       <c r="A101">
         <v>2020</v>
       </c>
@@ -8590,7 +10052,7 @@
         <v>13.5</v>
       </c>
       <c r="I101" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19.383333333333329</v>
       </c>
       <c r="K101" s="10">
@@ -8633,15 +10095,29 @@
         <v>983</v>
       </c>
       <c r="X101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="Y101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>557</v>
       </c>
-    </row>
-    <row r="102" spans="1:25" ht="15" thickBot="1">
+      <c r="AA101">
+        <f t="shared" si="7"/>
+        <v>12.507156666666663</v>
+      </c>
+      <c r="AB101">
+        <f t="shared" si="8"/>
+        <v>12.747156666666664</v>
+      </c>
+      <c r="AC101" s="41">
+        <v>804</v>
+      </c>
+      <c r="AD101">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="102" spans="1:30" ht="15" thickBot="1">
       <c r="A102">
         <v>2021</v>
       </c>
@@ -8667,7 +10143,7 @@
         <v>14.1</v>
       </c>
       <c r="I102" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18.066666666666666</v>
       </c>
       <c r="K102" s="23">
@@ -8710,12 +10186,26 @@
         <v>875</v>
       </c>
       <c r="X102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>105</v>
       </c>
       <c r="Y102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>624</v>
+      </c>
+      <c r="AA102">
+        <f t="shared" si="7"/>
+        <v>11.455368333333334</v>
+      </c>
+      <c r="AB102">
+        <f t="shared" si="8"/>
+        <v>11.455368333333334</v>
+      </c>
+      <c r="AC102" s="41">
+        <v>634</v>
+      </c>
+      <c r="AD102">
+        <v>0.96</v>
       </c>
     </row>
   </sheetData>
@@ -8728,8 +10218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EC36CD-A611-4488-BA35-43D34F546F10}">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8742,25 +10232,25 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="40" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>